<commit_message>
Ligeros ajustes del excel (TRELLO ESTABLECIDO)
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
@@ -167,9 +167,6 @@
     <t>Poner brujula sala 27</t>
   </si>
   <si>
-    <t>Implementar bloque especial empujable</t>
-  </si>
-  <si>
     <t>Crear prefab bloque especial</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>Sala 21 poner boomerang al clearear sala</t>
   </si>
   <si>
-    <t>boomerang</t>
-  </si>
-  <si>
     <t>sala 22 poner llave</t>
   </si>
   <si>
@@ -279,6 +273,12 @@
   </si>
   <si>
     <t>Iniciar Link sin objetos</t>
+  </si>
+  <si>
+    <t>Bloque especial empujable</t>
+  </si>
+  <si>
+    <t>Boomerang</t>
   </si>
 </sst>
 </file>
@@ -1032,66 +1032,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1105,197 +1045,257 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1885,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,36 +1915,36 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AG2" s="56"/>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="57"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
+      <c r="AA2" s="99"/>
+      <c r="AB2" s="99"/>
+      <c r="AC2" s="99"/>
+      <c r="AD2" s="99"/>
+      <c r="AE2" s="99"/>
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="99"/>
+      <c r="AH2" s="99"/>
+      <c r="AI2" s="99"/>
+      <c r="AJ2" s="99"/>
+      <c r="AK2" s="100"/>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
@@ -2057,11 +2057,11 @@
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="105" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="39" t="s">
@@ -2070,7 +2070,7 @@
       <c r="F4" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="69">
+      <c r="G4" s="47">
         <v>1</v>
       </c>
       <c r="H4" s="30">
@@ -2110,9 +2110,9 @@
       <c r="AK4" s="32"/>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="40" t="s">
@@ -2121,7 +2121,7 @@
       <c r="F5" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G5" s="48">
         <v>1</v>
       </c>
       <c r="H5" s="33">
@@ -2161,7 +2161,7 @@
       <c r="AK5" s="35"/>
     </row>
     <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="28" t="s">
         <v>37</v>
       </c>
@@ -2172,7 +2172,7 @@
       <c r="F6" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="70">
+      <c r="G6" s="48">
         <v>1</v>
       </c>
       <c r="H6" s="33">
@@ -2212,7 +2212,7 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="28" t="s">
         <v>39</v>
       </c>
@@ -2223,7 +2223,7 @@
       <c r="F7" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="70">
+      <c r="G7" s="48">
         <v>1</v>
       </c>
       <c r="H7" s="33">
@@ -2263,177 +2263,177 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="75"/>
-      <c r="C8" s="76" t="s">
+      <c r="B8" s="107"/>
+      <c r="C8" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="77" t="s">
+      <c r="D8" s="53"/>
+      <c r="E8" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="F8" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="78">
+      <c r="G8" s="55">
         <v>2</v>
       </c>
-      <c r="H8" s="79">
+      <c r="H8" s="56">
         <v>0.5</v>
       </c>
-      <c r="I8" s="80">
+      <c r="I8" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="79"/>
-      <c r="Y8" s="79"/>
-      <c r="Z8" s="79"/>
-      <c r="AA8" s="79"/>
-      <c r="AB8" s="79"/>
-      <c r="AC8" s="79"/>
-      <c r="AD8" s="79"/>
-      <c r="AE8" s="79"/>
-      <c r="AF8" s="79"/>
-      <c r="AG8" s="79"/>
-      <c r="AH8" s="81"/>
-      <c r="AI8" s="81"/>
-      <c r="AJ8" s="81"/>
-      <c r="AK8" s="82"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="56"/>
+      <c r="Y8" s="56"/>
+      <c r="Z8" s="56"/>
+      <c r="AA8" s="56"/>
+      <c r="AB8" s="56"/>
+      <c r="AC8" s="56"/>
+      <c r="AD8" s="56"/>
+      <c r="AE8" s="56"/>
+      <c r="AF8" s="56"/>
+      <c r="AG8" s="56"/>
+      <c r="AH8" s="58"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AK8" s="59"/>
     </row>
     <row r="9" spans="1:37" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="88" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="88" t="s">
+      <c r="D9" s="63"/>
+      <c r="E9" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="89">
+      <c r="G9" s="65">
         <v>2</v>
       </c>
-      <c r="H9" s="90">
+      <c r="H9" s="66">
         <v>0.2</v>
       </c>
       <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="90"/>
-      <c r="S9" s="90"/>
-      <c r="T9" s="90"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
-      <c r="AA9" s="90"/>
-      <c r="AB9" s="90"/>
-      <c r="AC9" s="90"/>
-      <c r="AD9" s="90"/>
-      <c r="AE9" s="90"/>
-      <c r="AF9" s="90"/>
-      <c r="AG9" s="90"/>
-      <c r="AH9" s="90"/>
-      <c r="AI9" s="90"/>
-      <c r="AJ9" s="90"/>
-      <c r="AK9" s="91"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="66"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="66"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="66"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="67"/>
     </row>
     <row r="10" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="84" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="84" t="s">
+      <c r="D10" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="50">
         <v>1</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="51">
         <v>0.25</v>
       </c>
-      <c r="I10" s="74">
+      <c r="I10" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="73"/>
-      <c r="V10" s="73"/>
-      <c r="W10" s="85"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="73"/>
-      <c r="AF10" s="73"/>
-      <c r="AG10" s="73"/>
-      <c r="AH10" s="73"/>
-      <c r="AI10" s="73"/>
-      <c r="AJ10" s="73"/>
-      <c r="AK10" s="86"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="51"/>
+      <c r="AA10" s="51"/>
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="51"/>
+      <c r="AD10" s="51"/>
+      <c r="AE10" s="51"/>
+      <c r="AF10" s="51"/>
+      <c r="AG10" s="51"/>
+      <c r="AH10" s="51"/>
+      <c r="AI10" s="51"/>
+      <c r="AJ10" s="51"/>
+      <c r="AK10" s="62"/>
     </row>
     <row r="11" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44"/>
-      <c r="C11" s="60"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F11" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="48">
         <v>1</v>
       </c>
       <c r="H11" s="33">
@@ -2473,122 +2473,122 @@
       <c r="AK11" s="36"/>
     </row>
     <row r="12" spans="1:37" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="96" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="96" t="s">
+      <c r="B12" s="127"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="97">
+      <c r="G12" s="70">
         <v>2</v>
       </c>
-      <c r="H12" s="98">
+      <c r="H12" s="71">
         <v>0.5</v>
       </c>
-      <c r="I12" s="99">
+      <c r="I12" s="72">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="98"/>
-      <c r="M12" s="98"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="98"/>
-      <c r="P12" s="98"/>
-      <c r="Q12" s="98"/>
-      <c r="R12" s="98"/>
-      <c r="S12" s="98"/>
-      <c r="T12" s="98"/>
-      <c r="U12" s="98"/>
-      <c r="V12" s="98"/>
-      <c r="W12" s="98"/>
-      <c r="X12" s="98"/>
-      <c r="Y12" s="98"/>
-      <c r="Z12" s="98"/>
-      <c r="AA12" s="98"/>
-      <c r="AB12" s="98"/>
-      <c r="AC12" s="98"/>
-      <c r="AD12" s="98"/>
-      <c r="AE12" s="98"/>
-      <c r="AF12" s="98"/>
-      <c r="AG12" s="98"/>
-      <c r="AH12" s="98"/>
-      <c r="AI12" s="98"/>
-      <c r="AJ12" s="98"/>
-      <c r="AK12" s="100"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
+      <c r="S12" s="71"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="71"/>
+      <c r="V12" s="71"/>
+      <c r="W12" s="71"/>
+      <c r="X12" s="71"/>
+      <c r="Y12" s="71"/>
+      <c r="Z12" s="71"/>
+      <c r="AA12" s="71"/>
+      <c r="AB12" s="71"/>
+      <c r="AC12" s="71"/>
+      <c r="AD12" s="71"/>
+      <c r="AE12" s="71"/>
+      <c r="AF12" s="71"/>
+      <c r="AG12" s="71"/>
+      <c r="AH12" s="71"/>
+      <c r="AI12" s="71"/>
+      <c r="AJ12" s="71"/>
+      <c r="AK12" s="73"/>
     </row>
     <row r="13" spans="1:37" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103" t="s">
+      <c r="C13" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="89">
+      <c r="G13" s="65">
         <v>1</v>
       </c>
-      <c r="H13" s="90">
+      <c r="H13" s="66">
         <v>0.1</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
-      <c r="AA13" s="90"/>
-      <c r="AB13" s="90"/>
-      <c r="AC13" s="90"/>
-      <c r="AD13" s="90"/>
-      <c r="AE13" s="104"/>
-      <c r="AF13" s="90"/>
-      <c r="AG13" s="90"/>
-      <c r="AH13" s="90"/>
-      <c r="AI13" s="90"/>
-      <c r="AJ13" s="90"/>
-      <c r="AK13" s="91"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="66"/>
+      <c r="S13" s="66"/>
+      <c r="T13" s="66"/>
+      <c r="U13" s="66"/>
+      <c r="V13" s="66"/>
+      <c r="W13" s="66"/>
+      <c r="X13" s="66"/>
+      <c r="Y13" s="66"/>
+      <c r="Z13" s="66"/>
+      <c r="AA13" s="66"/>
+      <c r="AB13" s="66"/>
+      <c r="AC13" s="66"/>
+      <c r="AD13" s="66"/>
+      <c r="AE13" s="77"/>
+      <c r="AF13" s="66"/>
+      <c r="AG13" s="66"/>
+      <c r="AH13" s="66"/>
+      <c r="AI13" s="66"/>
+      <c r="AJ13" s="66"/>
+      <c r="AK13" s="67"/>
     </row>
     <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="107" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107" t="s">
+      <c r="D14" s="78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="69">
+      <c r="G14" s="47">
         <v>3</v>
       </c>
       <c r="H14" s="30">
@@ -2611,7 +2611,7 @@
       <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="30"/>
-      <c r="W14" s="108"/>
+      <c r="W14" s="79"/>
       <c r="X14" s="30"/>
       <c r="Y14" s="30"/>
       <c r="Z14" s="30"/>
@@ -2625,19 +2625,19 @@
       <c r="AH14" s="30"/>
       <c r="AI14" s="30"/>
       <c r="AJ14" s="30"/>
-      <c r="AK14" s="109"/>
+      <c r="AK14" s="80"/>
     </row>
     <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="48"/>
-      <c r="C15" s="58"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="70">
+      <c r="G15" s="48">
         <v>2</v>
       </c>
       <c r="H15" s="33">
@@ -2677,16 +2677,16 @@
       <c r="AK15" s="38"/>
     </row>
     <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="48"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62" t="s">
+      <c r="B16" s="115"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="48">
         <v>2</v>
       </c>
       <c r="H16" s="33">
@@ -2726,16 +2726,16 @@
       <c r="AK16" s="38"/>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="62" t="s">
+      <c r="B17" s="115"/>
+      <c r="C17" s="111"/>
+      <c r="D17" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62" t="s">
+      <c r="E17" s="42"/>
+      <c r="F17" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="48">
         <v>2</v>
       </c>
       <c r="H17" s="33">
@@ -2775,8 +2775,8 @@
       <c r="AK17" s="38"/>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="48"/>
-      <c r="C18" s="58"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="111"/>
       <c r="D18" s="28" t="s">
         <v>34</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="F18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="70">
+      <c r="G18" s="48">
         <v>3</v>
       </c>
       <c r="H18" s="33">
@@ -2824,18 +2824,18 @@
       <c r="AK18" s="38"/>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="48"/>
-      <c r="C19" s="59" t="s">
+      <c r="B19" s="115"/>
+      <c r="C19" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62" t="s">
+      <c r="E19" s="42"/>
+      <c r="F19" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="70">
+      <c r="G19" s="48">
         <v>3</v>
       </c>
       <c r="H19" s="33">
@@ -2875,16 +2875,16 @@
       <c r="AK19" s="38"/>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="48"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="62" t="s">
+      <c r="B20" s="115"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62" t="s">
+      <c r="E20" s="42"/>
+      <c r="F20" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="70">
+      <c r="G20" s="48">
         <v>3</v>
       </c>
       <c r="H20" s="33">
@@ -2924,16 +2924,16 @@
       <c r="AK20" s="38"/>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="48"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="62" t="s">
+      <c r="B21" s="115"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62" t="s">
+      <c r="E21" s="42"/>
+      <c r="F21" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="70">
+      <c r="G21" s="48">
         <v>3</v>
       </c>
       <c r="H21" s="33">
@@ -2973,16 +2973,16 @@
       <c r="AK21" s="38"/>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="48"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="62" t="s">
+      <c r="B22" s="115"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62" t="s">
+      <c r="E22" s="42"/>
+      <c r="F22" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="48">
         <v>3</v>
       </c>
       <c r="H22" s="33">
@@ -3022,16 +3022,16 @@
       <c r="AK22" s="38"/>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="48"/>
-      <c r="C23" s="59"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="112"/>
       <c r="D23" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="41"/>
       <c r="F23" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="70">
+      <c r="G23" s="48">
         <v>3</v>
       </c>
       <c r="H23" s="33">
@@ -3071,16 +3071,16 @@
       <c r="AK23" s="38"/>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="48"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62" t="s">
+      <c r="B24" s="115"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="70">
+      <c r="G24" s="48">
         <v>3</v>
       </c>
       <c r="H24" s="33">
@@ -3120,16 +3120,16 @@
       <c r="AK24" s="38"/>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="48"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62" t="s">
+      <c r="B25" s="115"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="70">
+      <c r="G25" s="48">
         <v>3</v>
       </c>
       <c r="H25" s="33">
@@ -3169,16 +3169,16 @@
       <c r="AK25" s="38"/>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="48"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62" t="s">
+      <c r="B26" s="115"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G26" s="48">
         <v>3</v>
       </c>
       <c r="H26" s="33">
@@ -3218,16 +3218,16 @@
       <c r="AK26" s="38"/>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="48"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62" t="s">
+      <c r="B27" s="115"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="70">
+      <c r="G27" s="48">
         <v>3</v>
       </c>
       <c r="H27" s="33">
@@ -3267,16 +3267,16 @@
       <c r="AK27" s="38"/>
     </row>
     <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="48"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62" t="s">
+      <c r="B28" s="115"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="70">
+      <c r="G28" s="48">
         <v>3</v>
       </c>
       <c r="H28" s="33">
@@ -3316,16 +3316,16 @@
       <c r="AK28" s="38"/>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62" t="s">
+      <c r="B29" s="115"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="70">
+      <c r="G29" s="48">
         <v>3</v>
       </c>
       <c r="H29" s="33">
@@ -3365,18 +3365,18 @@
       <c r="AK29" s="38"/>
     </row>
     <row r="30" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="48"/>
-      <c r="C30" s="68" t="s">
-        <v>48</v>
+      <c r="B30" s="115"/>
+      <c r="C30" s="113" t="s">
+        <v>84</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G30" s="70">
+      <c r="G30" s="48">
         <v>2</v>
       </c>
       <c r="H30" s="33">
@@ -3416,16 +3416,16 @@
       <c r="AK30" s="38"/>
     </row>
     <row r="31" spans="2:37" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="48"/>
-      <c r="C31" s="68"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="113"/>
       <c r="D31" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="41"/>
       <c r="F31" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="70">
+      <c r="G31" s="48">
         <v>2</v>
       </c>
       <c r="H31" s="33">
@@ -3465,16 +3465,16 @@
       <c r="AK31" s="38"/>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="48"/>
-      <c r="C32" s="68"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="113"/>
       <c r="D32" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="41"/>
       <c r="F32" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="70">
+      <c r="G32" s="48">
         <v>1</v>
       </c>
       <c r="H32" s="33">
@@ -3514,16 +3514,16 @@
       <c r="AK32" s="38"/>
     </row>
     <row r="33" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="48"/>
-      <c r="C33" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62" t="s">
+      <c r="B33" s="115"/>
+      <c r="C33" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="70">
+      <c r="G33" s="48">
         <v>4</v>
       </c>
       <c r="H33" s="33">
@@ -3563,18 +3563,18 @@
       <c r="AK33" s="38"/>
     </row>
     <row r="34" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="48"/>
-      <c r="C34" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62" t="s">
+      <c r="B34" s="115"/>
+      <c r="C34" s="128" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="70">
+      <c r="G34" s="48">
         <v>5</v>
       </c>
       <c r="H34" s="33">
@@ -3614,16 +3614,16 @@
       <c r="AK34" s="38"/>
     </row>
     <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="48"/>
-      <c r="C35" s="46"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="129"/>
       <c r="D35" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E35" s="41"/>
       <c r="F35" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="70">
+      <c r="G35" s="48">
         <v>3</v>
       </c>
       <c r="H35" s="33">
@@ -3663,16 +3663,16 @@
       <c r="AK35" s="38"/>
     </row>
     <row r="36" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="48"/>
-      <c r="C36" s="46"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="129"/>
       <c r="D36" s="41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E36" s="41"/>
       <c r="F36" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="70">
+      <c r="G36" s="48">
         <v>5</v>
       </c>
       <c r="H36" s="33">
@@ -3712,16 +3712,16 @@
       <c r="AK36" s="38"/>
     </row>
     <row r="37" spans="2:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="48"/>
-      <c r="C37" s="46"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="129"/>
       <c r="D37" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="70">
+      <c r="G37" s="48">
         <v>4</v>
       </c>
       <c r="H37" s="33">
@@ -3761,16 +3761,16 @@
       <c r="AK37" s="38"/>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="48"/>
-      <c r="C38" s="47"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="130"/>
       <c r="D38" s="41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E38" s="41"/>
       <c r="F38" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="70">
+      <c r="G38" s="48">
         <v>2</v>
       </c>
       <c r="H38" s="33">
@@ -3810,18 +3810,18 @@
       <c r="AK38" s="38"/>
     </row>
     <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="48"/>
-      <c r="C39" s="67" t="s">
-        <v>65</v>
+      <c r="B39" s="115"/>
+      <c r="C39" s="120" t="s">
+        <v>63</v>
       </c>
       <c r="D39" s="41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" s="41"/>
       <c r="F39" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="70">
+      <c r="G39" s="48">
         <v>4</v>
       </c>
       <c r="H39" s="33">
@@ -3861,16 +3861,16 @@
       <c r="AK39" s="38"/>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="48"/>
-      <c r="C40" s="67"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="120"/>
       <c r="D40" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E40" s="41"/>
       <c r="F40" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="70">
+      <c r="G40" s="48">
         <v>4</v>
       </c>
       <c r="H40" s="33">
@@ -3910,16 +3910,16 @@
       <c r="AK40" s="38"/>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="48"/>
-      <c r="C41" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62" t="s">
+      <c r="B41" s="115"/>
+      <c r="C41" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="70">
+      <c r="G41" s="48">
         <v>1</v>
       </c>
       <c r="H41" s="33">
@@ -3959,70 +3959,70 @@
       <c r="AK41" s="38"/>
     </row>
     <row r="42" spans="2:37" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="110"/>
-      <c r="C42" s="111" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112" t="s">
+      <c r="B42" s="116"/>
+      <c r="C42" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="78">
+      <c r="G42" s="55">
         <v>6</v>
       </c>
-      <c r="H42" s="79">
+      <c r="H42" s="56">
         <v>3</v>
       </c>
-      <c r="I42" s="80">
+      <c r="I42" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="79"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="79"/>
-      <c r="N42" s="79"/>
-      <c r="O42" s="79"/>
-      <c r="P42" s="79"/>
-      <c r="Q42" s="79"/>
-      <c r="R42" s="79"/>
-      <c r="S42" s="79"/>
-      <c r="T42" s="113"/>
-      <c r="U42" s="113"/>
-      <c r="V42" s="113"/>
-      <c r="W42" s="113"/>
-      <c r="X42" s="79"/>
-      <c r="Y42" s="79"/>
-      <c r="Z42" s="79"/>
-      <c r="AA42" s="79"/>
-      <c r="AB42" s="79"/>
-      <c r="AC42" s="79"/>
-      <c r="AD42" s="79"/>
-      <c r="AE42" s="79"/>
-      <c r="AF42" s="79"/>
-      <c r="AG42" s="79"/>
-      <c r="AH42" s="113"/>
-      <c r="AI42" s="113"/>
-      <c r="AJ42" s="113"/>
-      <c r="AK42" s="114"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="56"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="56"/>
+      <c r="P42" s="56"/>
+      <c r="Q42" s="56"/>
+      <c r="R42" s="56"/>
+      <c r="S42" s="56"/>
+      <c r="T42" s="83"/>
+      <c r="U42" s="83"/>
+      <c r="V42" s="83"/>
+      <c r="W42" s="83"/>
+      <c r="X42" s="56"/>
+      <c r="Y42" s="56"/>
+      <c r="Z42" s="56"/>
+      <c r="AA42" s="56"/>
+      <c r="AB42" s="56"/>
+      <c r="AC42" s="56"/>
+      <c r="AD42" s="56"/>
+      <c r="AE42" s="56"/>
+      <c r="AF42" s="56"/>
+      <c r="AG42" s="56"/>
+      <c r="AH42" s="83"/>
+      <c r="AI42" s="83"/>
+      <c r="AJ42" s="83"/>
+      <c r="AK42" s="84"/>
     </row>
     <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="116" t="s">
+      <c r="C43" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="107"/>
-      <c r="E43" s="116"/>
-      <c r="F43" s="116" t="s">
+      <c r="D43" s="78"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="117">
+      <c r="G43" s="86">
         <v>3</v>
       </c>
-      <c r="H43" s="118">
+      <c r="H43" s="87">
         <v>0.75</v>
       </c>
       <c r="I43" s="18">
@@ -4056,10 +4056,10 @@
       <c r="AH43" s="30"/>
       <c r="AI43" s="30"/>
       <c r="AJ43" s="30"/>
-      <c r="AK43" s="119"/>
+      <c r="AK43" s="88"/>
     </row>
     <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="42"/>
+      <c r="B44" s="122"/>
       <c r="C44" s="29" t="s">
         <v>27</v>
       </c>
@@ -4068,7 +4068,7 @@
       <c r="F44" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="71">
+      <c r="G44" s="49">
         <v>3</v>
       </c>
       <c r="H44" s="4">
@@ -4108,8 +4108,8 @@
       <c r="AK44" s="36"/>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="42"/>
-      <c r="C45" s="43" t="s">
+      <c r="B45" s="122"/>
+      <c r="C45" s="124" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="28" t="s">
@@ -4119,7 +4119,7 @@
       <c r="F45" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="71">
+      <c r="G45" s="49">
         <v>3</v>
       </c>
       <c r="H45" s="4">
@@ -4159,67 +4159,67 @@
       <c r="AK45" s="36"/>
     </row>
     <row r="46" spans="2:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="120"/>
-      <c r="C46" s="121"/>
-      <c r="D46" s="76" t="s">
+      <c r="B46" s="123"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="122"/>
-      <c r="F46" s="122" t="s">
+      <c r="E46" s="89"/>
+      <c r="F46" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="123">
+      <c r="G46" s="90">
         <v>3</v>
       </c>
-      <c r="H46" s="124">
+      <c r="H46" s="91">
         <v>0.5</v>
       </c>
-      <c r="I46" s="80">
+      <c r="I46" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="79"/>
-      <c r="N46" s="79"/>
-      <c r="O46" s="79"/>
-      <c r="P46" s="79"/>
-      <c r="Q46" s="79"/>
-      <c r="R46" s="79"/>
-      <c r="S46" s="79"/>
-      <c r="T46" s="79"/>
-      <c r="U46" s="79"/>
-      <c r="V46" s="79"/>
-      <c r="W46" s="79"/>
-      <c r="X46" s="79"/>
-      <c r="Y46" s="79"/>
-      <c r="Z46" s="79"/>
-      <c r="AA46" s="79"/>
-      <c r="AB46" s="79"/>
-      <c r="AC46" s="79"/>
-      <c r="AD46" s="79"/>
-      <c r="AE46" s="79"/>
-      <c r="AF46" s="79"/>
-      <c r="AG46" s="79"/>
-      <c r="AH46" s="79"/>
-      <c r="AI46" s="79"/>
-      <c r="AJ46" s="79"/>
-      <c r="AK46" s="125"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="56"/>
+      <c r="V46" s="56"/>
+      <c r="W46" s="56"/>
+      <c r="X46" s="56"/>
+      <c r="Y46" s="56"/>
+      <c r="Z46" s="56"/>
+      <c r="AA46" s="56"/>
+      <c r="AB46" s="56"/>
+      <c r="AC46" s="56"/>
+      <c r="AD46" s="56"/>
+      <c r="AE46" s="56"/>
+      <c r="AF46" s="56"/>
+      <c r="AG46" s="56"/>
+      <c r="AH46" s="56"/>
+      <c r="AI46" s="56"/>
+      <c r="AJ46" s="56"/>
+      <c r="AK46" s="92"/>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="105" t="s">
+      <c r="B47" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="126" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="127"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="128" t="s">
+      <c r="C47" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="94"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="G47" s="69">
+      <c r="G47" s="47">
         <v>2</v>
       </c>
       <c r="H47" s="30">
@@ -4256,19 +4256,19 @@
       <c r="AH47" s="30"/>
       <c r="AI47" s="30"/>
       <c r="AJ47" s="30"/>
-      <c r="AK47" s="119"/>
+      <c r="AK47" s="88"/>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="48"/>
-      <c r="C48" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="62"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64" t="s">
+      <c r="B48" s="115"/>
+      <c r="C48" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="42"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G48" s="70">
+      <c r="G48" s="48">
         <v>1</v>
       </c>
       <c r="H48" s="33">
@@ -4308,16 +4308,16 @@
       <c r="AK48" s="36"/>
     </row>
     <row r="49" spans="2:37" ht="21" x14ac:dyDescent="0.3">
-      <c r="B49" s="48"/>
-      <c r="C49" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="62"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64" t="s">
+      <c r="B49" s="115"/>
+      <c r="C49" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="42"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G49" s="70">
+      <c r="G49" s="48">
         <v>1</v>
       </c>
       <c r="H49" s="33">
@@ -4357,63 +4357,63 @@
       <c r="AK49" s="38"/>
     </row>
     <row r="50" spans="2:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="110"/>
-      <c r="C50" s="129" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="130"/>
-      <c r="E50" s="129"/>
-      <c r="F50" s="129" t="s">
+      <c r="B50" s="116"/>
+      <c r="C50" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="97"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="78">
+      <c r="G50" s="55">
         <v>1</v>
       </c>
-      <c r="H50" s="79">
+      <c r="H50" s="56">
         <v>1</v>
       </c>
-      <c r="I50" s="80">
+      <c r="I50" s="57">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J50" s="79"/>
-      <c r="K50" s="79"/>
-      <c r="L50" s="79"/>
-      <c r="M50" s="79"/>
-      <c r="N50" s="79"/>
-      <c r="O50" s="113"/>
-      <c r="P50" s="113"/>
-      <c r="Q50" s="113"/>
-      <c r="R50" s="113"/>
-      <c r="S50" s="113"/>
-      <c r="T50" s="113"/>
-      <c r="U50" s="113"/>
-      <c r="V50" s="113"/>
-      <c r="W50" s="113"/>
-      <c r="X50" s="79"/>
-      <c r="Y50" s="79"/>
-      <c r="Z50" s="79"/>
-      <c r="AA50" s="79"/>
-      <c r="AB50" s="79"/>
-      <c r="AC50" s="113"/>
-      <c r="AD50" s="113"/>
-      <c r="AE50" s="113"/>
-      <c r="AF50" s="113"/>
-      <c r="AG50" s="113"/>
-      <c r="AH50" s="113"/>
-      <c r="AI50" s="113"/>
-      <c r="AJ50" s="113"/>
-      <c r="AK50" s="114"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="56"/>
+      <c r="O50" s="83"/>
+      <c r="P50" s="83"/>
+      <c r="Q50" s="83"/>
+      <c r="R50" s="83"/>
+      <c r="S50" s="83"/>
+      <c r="T50" s="83"/>
+      <c r="U50" s="83"/>
+      <c r="V50" s="83"/>
+      <c r="W50" s="83"/>
+      <c r="X50" s="56"/>
+      <c r="Y50" s="56"/>
+      <c r="Z50" s="56"/>
+      <c r="AA50" s="56"/>
+      <c r="AB50" s="56"/>
+      <c r="AC50" s="83"/>
+      <c r="AD50" s="83"/>
+      <c r="AE50" s="83"/>
+      <c r="AF50" s="83"/>
+      <c r="AG50" s="83"/>
+      <c r="AH50" s="83"/>
+      <c r="AI50" s="83"/>
+      <c r="AJ50" s="83"/>
+      <c r="AK50" s="84"/>
     </row>
     <row r="51" spans="2:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
+      <c r="C51" s="109"/>
+      <c r="D51" s="109"/>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109"/>
+      <c r="G51" s="109"/>
       <c r="H51" s="14">
         <f t="shared" ref="H51:W51" si="1">SUM(H4:H50)</f>
         <v>32.299999999999997</v>
@@ -4488,22 +4488,22 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="49" t="s">
+      <c r="J52" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="50"/>
-      <c r="O52" s="50"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="50"/>
-      <c r="R52" s="50"/>
-      <c r="S52" s="50"/>
-      <c r="T52" s="50"/>
-      <c r="U52" s="50"/>
-      <c r="V52" s="50"/>
-      <c r="W52" s="51"/>
+      <c r="K52" s="103"/>
+      <c r="L52" s="103"/>
+      <c r="M52" s="103"/>
+      <c r="N52" s="103"/>
+      <c r="O52" s="103"/>
+      <c r="P52" s="103"/>
+      <c r="Q52" s="103"/>
+      <c r="R52" s="103"/>
+      <c r="S52" s="103"/>
+      <c r="T52" s="103"/>
+      <c r="U52" s="103"/>
+      <c r="V52" s="103"/>
+      <c r="W52" s="104"/>
     </row>
     <row r="53" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="20" t="s">
@@ -4547,10 +4547,10 @@
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="55" t="s">
+      <c r="H54" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="I54" s="61"/>
+      <c r="I54" s="101"/>
       <c r="J54" s="10">
         <f>H51-J51</f>
         <v>32.299999999999997</v>
@@ -4650,27 +4650,27 @@
         <v>11.85</v>
       </c>
       <c r="F56" s="3"/>
-      <c r="H56" s="55" t="s">
+      <c r="H56" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="I56" s="56"/>
-      <c r="J56" s="55">
+      <c r="I56" s="99"/>
+      <c r="J56" s="98">
         <f>H51-I51</f>
         <v>32.299999999999997</v>
       </c>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
-      <c r="O56" s="56"/>
-      <c r="P56" s="56"/>
-      <c r="Q56" s="56"/>
-      <c r="R56" s="56"/>
-      <c r="S56" s="56"/>
-      <c r="T56" s="56"/>
-      <c r="U56" s="56"/>
-      <c r="V56" s="56"/>
-      <c r="W56" s="57"/>
+      <c r="K56" s="99"/>
+      <c r="L56" s="99"/>
+      <c r="M56" s="99"/>
+      <c r="N56" s="99"/>
+      <c r="O56" s="99"/>
+      <c r="P56" s="99"/>
+      <c r="Q56" s="99"/>
+      <c r="R56" s="99"/>
+      <c r="S56" s="99"/>
+      <c r="T56" s="99"/>
+      <c r="U56" s="99"/>
+      <c r="V56" s="99"/>
+      <c r="W56" s="100"/>
     </row>
     <row r="57" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
@@ -4750,12 +4750,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J56:W56"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J52:W52"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B51:G51"/>
     <mergeCell ref="J2:AK2"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="C19:C29"/>
@@ -4768,6 +4762,12 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C34:C38"/>
     <mergeCell ref="B14:B42"/>
+    <mergeCell ref="J56:W56"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="J52:W52"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado excel + Link empieza sin objetos
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MSI-D\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +447,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -909,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1186,10 +1192,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1246,9 +1309,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1261,58 +1321,19 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1478,85 +1499,85 @@
                   <c:v>32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>32.200699999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>32.084699999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>31.835699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>31.835699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>32.049999999999997</c:v>
+                  <c:v>31.535699999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,7 +1644,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1755,6 +1775,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1790,6 +1827,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1968,28 +2022,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="55.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
@@ -1997,39 +2051,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="96" t="s">
+    <row r="2" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="97"/>
-      <c r="AH2" s="97"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="98"/>
-    </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="111"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="111"/>
+      <c r="AF2" s="111"/>
+      <c r="AG2" s="111"/>
+      <c r="AH2" s="111"/>
+      <c r="AI2" s="111"/>
+      <c r="AJ2" s="111"/>
+      <c r="AK2" s="117"/>
+    </row>
+    <row r="3" spans="1:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2139,8 +2193,8 @@
         <v>43109</v>
       </c>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="122" t="s">
+    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="112" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="38" t="s">
@@ -2163,11 +2217,21 @@
         <f>SUM(J4:W4)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="139">
+        <v>0</v>
+      </c>
+      <c r="K4" s="139">
+        <v>0</v>
+      </c>
+      <c r="L4" s="139">
+        <v>0</v>
+      </c>
+      <c r="M4" s="139">
+        <v>0</v>
+      </c>
+      <c r="N4" s="139">
+        <v>0</v>
+      </c>
       <c r="O4" s="29"/>
       <c r="P4" s="29"/>
       <c r="Q4" s="30"/>
@@ -2192,8 +2256,8 @@
       <c r="AJ4" s="30"/>
       <c r="AK4" s="31"/>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="116"/>
+    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="113"/>
       <c r="C5" s="27" t="s">
         <v>74</v>
       </c>
@@ -2214,11 +2278,21 @@
         <f t="shared" ref="I5:I50" si="0">SUM(J5:W5)</f>
         <v>0</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="J5" s="102">
+        <v>0</v>
+      </c>
+      <c r="K5" s="102">
+        <v>0</v>
+      </c>
+      <c r="L5" s="102">
+        <v>0</v>
+      </c>
+      <c r="M5" s="102">
+        <v>0</v>
+      </c>
+      <c r="N5" s="102">
+        <v>0</v>
+      </c>
       <c r="O5" s="32"/>
       <c r="P5" s="32"/>
       <c r="Q5" s="33"/>
@@ -2243,8 +2317,8 @@
       <c r="AJ5" s="33"/>
       <c r="AK5" s="34"/>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="116"/>
+    <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="113"/>
       <c r="C6" s="27" t="s">
         <v>37</v>
       </c>
@@ -2265,11 +2339,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
+      <c r="J6" s="102">
+        <v>0</v>
+      </c>
+      <c r="K6" s="102">
+        <v>0</v>
+      </c>
+      <c r="L6" s="102">
+        <v>0</v>
+      </c>
+      <c r="M6" s="102">
+        <v>0</v>
+      </c>
+      <c r="N6" s="102">
+        <v>0</v>
+      </c>
       <c r="O6" s="32"/>
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
@@ -2294,8 +2378,8 @@
       <c r="AJ6" s="33"/>
       <c r="AK6" s="34"/>
     </row>
-    <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="116"/>
+    <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="113"/>
       <c r="C7" s="27" t="s">
         <v>39</v>
       </c>
@@ -2316,11 +2400,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
+      <c r="J7" s="102">
+        <v>0</v>
+      </c>
+      <c r="K7" s="102">
+        <v>0</v>
+      </c>
+      <c r="L7" s="102">
+        <v>0</v>
+      </c>
+      <c r="M7" s="102">
+        <v>0</v>
+      </c>
+      <c r="N7" s="102">
+        <v>0</v>
+      </c>
       <c r="O7" s="32"/>
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
@@ -2345,8 +2439,8 @@
       <c r="AJ7" s="33"/>
       <c r="AK7" s="34"/>
     </row>
-    <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="123"/>
+    <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="114"/>
       <c r="C8" s="52" t="s">
         <v>40</v>
       </c>
@@ -2367,11 +2461,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
+      <c r="J8" s="140">
+        <v>0</v>
+      </c>
+      <c r="K8" s="140">
+        <v>0</v>
+      </c>
+      <c r="L8" s="140">
+        <v>0</v>
+      </c>
+      <c r="M8" s="140">
+        <v>0</v>
+      </c>
+      <c r="N8" s="140">
+        <v>0</v>
+      </c>
       <c r="O8" s="55"/>
       <c r="P8" s="55"/>
       <c r="Q8" s="55"/>
@@ -2396,7 +2500,7 @@
       <c r="AJ8" s="57"/>
       <c r="AK8" s="58"/>
     </row>
-    <row r="9" spans="1:37" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="65" t="s">
         <v>41</v>
       </c>
@@ -2420,11 +2524,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
+      <c r="J9" s="141">
+        <v>0</v>
+      </c>
+      <c r="K9" s="141">
+        <v>0</v>
+      </c>
+      <c r="L9" s="141">
+        <v>0</v>
+      </c>
+      <c r="M9" s="141">
+        <v>0</v>
+      </c>
+      <c r="N9" s="141">
+        <v>0</v>
+      </c>
       <c r="O9" s="63"/>
       <c r="P9" s="63"/>
       <c r="Q9" s="63"/>
@@ -2449,11 +2563,11 @@
       <c r="AJ9" s="63"/>
       <c r="AK9" s="64"/>
     </row>
-    <row r="10" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="115" t="s">
+    <row r="10" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="125" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="59" t="s">
@@ -2475,50 +2589,50 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J10" s="131">
-        <v>0</v>
-      </c>
-      <c r="K10" s="131">
-        <v>0</v>
-      </c>
-      <c r="L10" s="131">
-        <v>0</v>
-      </c>
-      <c r="M10" s="131">
-        <v>0</v>
-      </c>
-      <c r="N10" s="131">
-        <v>0</v>
-      </c>
-      <c r="O10" s="133">
+      <c r="J10" s="101">
+        <v>0</v>
+      </c>
+      <c r="K10" s="101">
+        <v>0</v>
+      </c>
+      <c r="L10" s="101">
+        <v>0</v>
+      </c>
+      <c r="M10" s="101">
+        <v>0</v>
+      </c>
+      <c r="N10" s="101">
+        <v>0</v>
+      </c>
+      <c r="O10" s="103">
         <v>0.15</v>
       </c>
-      <c r="P10" s="133"/>
-      <c r="Q10" s="133"/>
-      <c r="R10" s="133"/>
-      <c r="S10" s="133"/>
-      <c r="T10" s="133"/>
-      <c r="U10" s="133"/>
-      <c r="V10" s="133"/>
-      <c r="W10" s="134"/>
-      <c r="X10" s="133"/>
-      <c r="Y10" s="133"/>
-      <c r="Z10" s="133"/>
-      <c r="AA10" s="133"/>
-      <c r="AB10" s="133"/>
-      <c r="AC10" s="133"/>
-      <c r="AD10" s="133"/>
-      <c r="AE10" s="133"/>
-      <c r="AF10" s="133"/>
-      <c r="AG10" s="133"/>
-      <c r="AH10" s="133"/>
-      <c r="AI10" s="133"/>
-      <c r="AJ10" s="133"/>
-      <c r="AK10" s="135"/>
-    </row>
-    <row r="11" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="116"/>
-      <c r="C11" s="107"/>
+      <c r="P10" s="103"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="103"/>
+      <c r="T10" s="103"/>
+      <c r="U10" s="103"/>
+      <c r="V10" s="103"/>
+      <c r="W10" s="104"/>
+      <c r="X10" s="103"/>
+      <c r="Y10" s="103"/>
+      <c r="Z10" s="103"/>
+      <c r="AA10" s="103"/>
+      <c r="AB10" s="103"/>
+      <c r="AC10" s="103"/>
+      <c r="AD10" s="103"/>
+      <c r="AE10" s="103"/>
+      <c r="AF10" s="103"/>
+      <c r="AG10" s="103"/>
+      <c r="AH10" s="103"/>
+      <c r="AI10" s="103"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="105"/>
+    </row>
+    <row r="11" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="113"/>
+      <c r="C11" s="126"/>
       <c r="D11" s="40" t="s">
         <v>61</v>
       </c>
@@ -2538,50 +2652,50 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="J11" s="132">
-        <v>0</v>
-      </c>
-      <c r="K11" s="132">
-        <v>0</v>
-      </c>
-      <c r="L11" s="132">
-        <v>0</v>
-      </c>
-      <c r="M11" s="132">
-        <v>0</v>
-      </c>
-      <c r="N11" s="132">
-        <v>0</v>
-      </c>
-      <c r="O11" s="136">
+      <c r="J11" s="102">
+        <v>0</v>
+      </c>
+      <c r="K11" s="102">
+        <v>0</v>
+      </c>
+      <c r="L11" s="102">
+        <v>0</v>
+      </c>
+      <c r="M11" s="102">
+        <v>0</v>
+      </c>
+      <c r="N11" s="102">
+        <v>0</v>
+      </c>
+      <c r="O11" s="106">
         <v>0.1</v>
       </c>
-      <c r="P11" s="136"/>
-      <c r="Q11" s="136"/>
-      <c r="R11" s="136"/>
-      <c r="S11" s="136"/>
-      <c r="T11" s="136"/>
-      <c r="U11" s="136"/>
-      <c r="V11" s="136"/>
-      <c r="W11" s="136"/>
-      <c r="X11" s="136"/>
-      <c r="Y11" s="136"/>
-      <c r="Z11" s="136"/>
-      <c r="AA11" s="136"/>
-      <c r="AB11" s="136"/>
-      <c r="AC11" s="136"/>
-      <c r="AD11" s="136"/>
-      <c r="AE11" s="136"/>
-      <c r="AF11" s="136"/>
-      <c r="AG11" s="136"/>
-      <c r="AH11" s="136"/>
-      <c r="AI11" s="136"/>
-      <c r="AJ11" s="136"/>
-      <c r="AK11" s="137"/>
-    </row>
-    <row r="12" spans="1:37" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="117"/>
-      <c r="C12" s="108"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
+      <c r="T11" s="106"/>
+      <c r="U11" s="106"/>
+      <c r="V11" s="106"/>
+      <c r="W11" s="106"/>
+      <c r="X11" s="106"/>
+      <c r="Y11" s="106"/>
+      <c r="Z11" s="106"/>
+      <c r="AA11" s="106"/>
+      <c r="AB11" s="106"/>
+      <c r="AC11" s="106"/>
+      <c r="AD11" s="106"/>
+      <c r="AE11" s="106"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="106"/>
+      <c r="AH11" s="106"/>
+      <c r="AI11" s="106"/>
+      <c r="AJ11" s="106"/>
+      <c r="AK11" s="107"/>
+    </row>
+    <row r="12" spans="1:37" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="135"/>
+      <c r="C12" s="127"/>
       <c r="D12" s="66" t="s">
         <v>62</v>
       </c>
@@ -2601,19 +2715,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="138">
-        <v>0</v>
-      </c>
-      <c r="K12" s="138">
-        <v>0</v>
-      </c>
-      <c r="L12" s="138">
-        <v>0</v>
-      </c>
-      <c r="M12" s="138">
-        <v>0</v>
-      </c>
-      <c r="N12" s="138">
+      <c r="J12" s="108">
+        <v>0</v>
+      </c>
+      <c r="K12" s="108">
+        <v>0</v>
+      </c>
+      <c r="L12" s="108">
+        <v>0</v>
+      </c>
+      <c r="M12" s="108">
+        <v>0</v>
+      </c>
+      <c r="N12" s="108">
         <v>0</v>
       </c>
       <c r="O12" s="68"/>
@@ -2640,7 +2754,7 @@
       <c r="AJ12" s="68"/>
       <c r="AK12" s="70"/>
     </row>
-    <row r="13" spans="1:37" ht="22.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:37" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="71" t="s">
         <v>22</v>
       </c>
@@ -2660,13 +2774,23 @@
       </c>
       <c r="I13" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="63"/>
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="J13" s="141">
+        <v>0</v>
+      </c>
+      <c r="K13" s="143">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="L13" s="143">
+        <v>0</v>
+      </c>
+      <c r="M13" s="143">
+        <v>0</v>
+      </c>
+      <c r="N13" s="143">
+        <v>0</v>
+      </c>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
       <c r="Q13" s="74"/>
@@ -2691,11 +2815,11 @@
       <c r="AJ13" s="63"/>
       <c r="AK13" s="64"/>
     </row>
-    <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="103" t="s">
+    <row r="14" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="118" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="75" t="s">
@@ -2715,11 +2839,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
+      <c r="J14" s="139">
+        <v>0</v>
+      </c>
+      <c r="K14" s="139">
+        <v>0</v>
+      </c>
+      <c r="L14" s="139">
+        <v>0</v>
+      </c>
+      <c r="M14" s="139">
+        <v>0</v>
+      </c>
+      <c r="N14" s="139">
+        <v>0</v>
+      </c>
       <c r="O14" s="29"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
@@ -2744,9 +2878,9 @@
       <c r="AJ14" s="29"/>
       <c r="AK14" s="77"/>
     </row>
-    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="104"/>
-      <c r="C15" s="100"/>
+    <row r="15" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="123"/>
+      <c r="C15" s="119"/>
       <c r="D15" s="27" t="s">
         <v>76</v>
       </c>
@@ -2764,11 +2898,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="J15" s="102">
+        <v>0</v>
+      </c>
+      <c r="K15" s="102">
+        <v>0</v>
+      </c>
+      <c r="L15" s="102">
+        <v>0</v>
+      </c>
+      <c r="M15" s="102">
+        <v>0</v>
+      </c>
+      <c r="N15" s="102">
+        <v>0</v>
+      </c>
       <c r="O15" s="32"/>
       <c r="P15" s="32"/>
       <c r="Q15" s="32"/>
@@ -2793,9 +2937,9 @@
       <c r="AJ15" s="32"/>
       <c r="AK15" s="37"/>
     </row>
-    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="104"/>
-      <c r="C16" s="100"/>
+    <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="123"/>
+      <c r="C16" s="119"/>
       <c r="D16" s="41" t="s">
         <v>51</v>
       </c>
@@ -2813,11 +2957,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="J16" s="102">
+        <v>0</v>
+      </c>
+      <c r="K16" s="102">
+        <v>0</v>
+      </c>
+      <c r="L16" s="102">
+        <v>0</v>
+      </c>
+      <c r="M16" s="102">
+        <v>0</v>
+      </c>
+      <c r="N16" s="102">
+        <v>0</v>
+      </c>
       <c r="O16" s="32"/>
       <c r="P16" s="32"/>
       <c r="Q16" s="32"/>
@@ -2842,9 +2996,9 @@
       <c r="AJ16" s="36"/>
       <c r="AK16" s="37"/>
     </row>
-    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="104"/>
-      <c r="C17" s="100"/>
+    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="123"/>
+      <c r="C17" s="119"/>
       <c r="D17" s="41" t="s">
         <v>33</v>
       </c>
@@ -2862,11 +3016,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="J17" s="102">
+        <v>0</v>
+      </c>
+      <c r="K17" s="102">
+        <v>0</v>
+      </c>
+      <c r="L17" s="102">
+        <v>0</v>
+      </c>
+      <c r="M17" s="102">
+        <v>0</v>
+      </c>
+      <c r="N17" s="102">
+        <v>0</v>
+      </c>
       <c r="O17" s="32"/>
       <c r="P17" s="32"/>
       <c r="Q17" s="32"/>
@@ -2891,9 +3055,9 @@
       <c r="AJ17" s="36"/>
       <c r="AK17" s="37"/>
     </row>
-    <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="104"/>
-      <c r="C18" s="100"/>
+    <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="123"/>
+      <c r="C18" s="119"/>
       <c r="D18" s="27" t="s">
         <v>34</v>
       </c>
@@ -2911,11 +3075,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
+      <c r="J18" s="102">
+        <v>0</v>
+      </c>
+      <c r="K18" s="102">
+        <v>0</v>
+      </c>
+      <c r="L18" s="102">
+        <v>0</v>
+      </c>
+      <c r="M18" s="102">
+        <v>0</v>
+      </c>
+      <c r="N18" s="102">
+        <v>0</v>
+      </c>
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
@@ -2940,9 +3114,9 @@
       <c r="AJ18" s="36"/>
       <c r="AK18" s="37"/>
     </row>
-    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="104"/>
-      <c r="C19" s="101" t="s">
+    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="123"/>
+      <c r="C19" s="120" t="s">
         <v>43</v>
       </c>
       <c r="D19" s="41" t="s">
@@ -2962,11 +3136,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
+      <c r="J19" s="102">
+        <v>0</v>
+      </c>
+      <c r="K19" s="102">
+        <v>0</v>
+      </c>
+      <c r="L19" s="102">
+        <v>0</v>
+      </c>
+      <c r="M19" s="102">
+        <v>0</v>
+      </c>
+      <c r="N19" s="102">
+        <v>0</v>
+      </c>
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
@@ -2991,9 +3175,9 @@
       <c r="AJ19" s="36"/>
       <c r="AK19" s="37"/>
     </row>
-    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="104"/>
-      <c r="C20" s="101"/>
+    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="123"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="41" t="s">
         <v>45</v>
       </c>
@@ -3011,11 +3195,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
+      <c r="J20" s="102">
+        <v>0</v>
+      </c>
+      <c r="K20" s="102">
+        <v>0</v>
+      </c>
+      <c r="L20" s="102">
+        <v>0</v>
+      </c>
+      <c r="M20" s="102">
+        <v>0</v>
+      </c>
+      <c r="N20" s="102">
+        <v>0</v>
+      </c>
       <c r="O20" s="32"/>
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
@@ -3040,9 +3234,9 @@
       <c r="AJ20" s="36"/>
       <c r="AK20" s="37"/>
     </row>
-    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="104"/>
-      <c r="C21" s="101"/>
+    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="123"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="41" t="s">
         <v>46</v>
       </c>
@@ -3060,11 +3254,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="J21" s="102">
+        <v>0</v>
+      </c>
+      <c r="K21" s="102">
+        <v>0</v>
+      </c>
+      <c r="L21" s="102">
+        <v>0</v>
+      </c>
+      <c r="M21" s="102">
+        <v>0</v>
+      </c>
+      <c r="N21" s="102">
+        <v>0</v>
+      </c>
       <c r="O21" s="32"/>
       <c r="P21" s="32"/>
       <c r="Q21" s="32"/>
@@ -3089,9 +3293,9 @@
       <c r="AJ21" s="36"/>
       <c r="AK21" s="37"/>
     </row>
-    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="104"/>
-      <c r="C22" s="101"/>
+    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="123"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="41" t="s">
         <v>47</v>
       </c>
@@ -3109,11 +3313,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
+      <c r="J22" s="102">
+        <v>0</v>
+      </c>
+      <c r="K22" s="102">
+        <v>0</v>
+      </c>
+      <c r="L22" s="102">
+        <v>0</v>
+      </c>
+      <c r="M22" s="102">
+        <v>0</v>
+      </c>
+      <c r="N22" s="102">
+        <v>0</v>
+      </c>
       <c r="O22" s="32"/>
       <c r="P22" s="32"/>
       <c r="Q22" s="32"/>
@@ -3138,9 +3352,9 @@
       <c r="AJ22" s="36"/>
       <c r="AK22" s="37"/>
     </row>
-    <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="104"/>
-      <c r="C23" s="101"/>
+    <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="123"/>
+      <c r="C23" s="120"/>
       <c r="D23" s="40" t="s">
         <v>49</v>
       </c>
@@ -3158,11 +3372,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
+      <c r="J23" s="102">
+        <v>0</v>
+      </c>
+      <c r="K23" s="102">
+        <v>0</v>
+      </c>
+      <c r="L23" s="102">
+        <v>0</v>
+      </c>
+      <c r="M23" s="102">
+        <v>0</v>
+      </c>
+      <c r="N23" s="102">
+        <v>0</v>
+      </c>
       <c r="O23" s="32"/>
       <c r="P23" s="32"/>
       <c r="Q23" s="32"/>
@@ -3187,9 +3411,9 @@
       <c r="AJ23" s="36"/>
       <c r="AK23" s="37"/>
     </row>
-    <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="104"/>
-      <c r="C24" s="101"/>
+    <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="123"/>
+      <c r="C24" s="120"/>
       <c r="D24" s="41" t="s">
         <v>52</v>
       </c>
@@ -3207,11 +3431,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
+      <c r="J24" s="102">
+        <v>0</v>
+      </c>
+      <c r="K24" s="102">
+        <v>0</v>
+      </c>
+      <c r="L24" s="102">
+        <v>0</v>
+      </c>
+      <c r="M24" s="102">
+        <v>0</v>
+      </c>
+      <c r="N24" s="102">
+        <v>0</v>
+      </c>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
       <c r="Q24" s="32"/>
@@ -3236,9 +3470,9 @@
       <c r="AJ24" s="36"/>
       <c r="AK24" s="37"/>
     </row>
-    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="104"/>
-      <c r="C25" s="101"/>
+    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="123"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="41" t="s">
         <v>53</v>
       </c>
@@ -3256,11 +3490,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="J25" s="102">
+        <v>0</v>
+      </c>
+      <c r="K25" s="102">
+        <v>0</v>
+      </c>
+      <c r="L25" s="102">
+        <v>0</v>
+      </c>
+      <c r="M25" s="102">
+        <v>0</v>
+      </c>
+      <c r="N25" s="102">
+        <v>0</v>
+      </c>
       <c r="O25" s="32"/>
       <c r="P25" s="32"/>
       <c r="Q25" s="32"/>
@@ -3285,9 +3529,9 @@
       <c r="AJ25" s="36"/>
       <c r="AK25" s="37"/>
     </row>
-    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="104"/>
-      <c r="C26" s="101"/>
+    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="123"/>
+      <c r="C26" s="120"/>
       <c r="D26" s="41" t="s">
         <v>54</v>
       </c>
@@ -3305,11 +3549,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
+      <c r="J26" s="102">
+        <v>0</v>
+      </c>
+      <c r="K26" s="102">
+        <v>0</v>
+      </c>
+      <c r="L26" s="102">
+        <v>0</v>
+      </c>
+      <c r="M26" s="102">
+        <v>0</v>
+      </c>
+      <c r="N26" s="102">
+        <v>0</v>
+      </c>
       <c r="O26" s="32"/>
       <c r="P26" s="32"/>
       <c r="Q26" s="32"/>
@@ -3334,9 +3588,9 @@
       <c r="AJ26" s="36"/>
       <c r="AK26" s="37"/>
     </row>
-    <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="104"/>
-      <c r="C27" s="101"/>
+    <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="123"/>
+      <c r="C27" s="120"/>
       <c r="D27" s="41" t="s">
         <v>58</v>
       </c>
@@ -3352,13 +3606,23 @@
       </c>
       <c r="I27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="J27" s="102">
+        <v>0</v>
+      </c>
+      <c r="K27" s="106">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L27" s="106">
+        <v>0</v>
+      </c>
+      <c r="M27" s="106">
+        <v>0</v>
+      </c>
+      <c r="N27" s="106">
+        <v>0</v>
+      </c>
       <c r="O27" s="32"/>
       <c r="P27" s="32"/>
       <c r="Q27" s="32"/>
@@ -3383,9 +3647,9 @@
       <c r="AJ27" s="36"/>
       <c r="AK27" s="37"/>
     </row>
-    <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="104"/>
-      <c r="C28" s="101"/>
+    <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="123"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="41" t="s">
         <v>56</v>
       </c>
@@ -3403,11 +3667,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
+      <c r="J28" s="102">
+        <v>0</v>
+      </c>
+      <c r="K28" s="102">
+        <v>0</v>
+      </c>
+      <c r="L28" s="102">
+        <v>0</v>
+      </c>
+      <c r="M28" s="102">
+        <v>0</v>
+      </c>
+      <c r="N28" s="102">
+        <v>0</v>
+      </c>
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
       <c r="Q28" s="32"/>
@@ -3432,9 +3706,9 @@
       <c r="AJ28" s="36"/>
       <c r="AK28" s="37"/>
     </row>
-    <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="104"/>
-      <c r="C29" s="101"/>
+    <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="123"/>
+      <c r="C29" s="120"/>
       <c r="D29" s="41" t="s">
         <v>57</v>
       </c>
@@ -3452,11 +3726,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
+      <c r="J29" s="102">
+        <v>0</v>
+      </c>
+      <c r="K29" s="102">
+        <v>0</v>
+      </c>
+      <c r="L29" s="102">
+        <v>0</v>
+      </c>
+      <c r="M29" s="102">
+        <v>0</v>
+      </c>
+      <c r="N29" s="102">
+        <v>0</v>
+      </c>
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
       <c r="Q29" s="32"/>
@@ -3481,9 +3765,9 @@
       <c r="AJ29" s="36"/>
       <c r="AK29" s="37"/>
     </row>
-    <row r="30" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="104"/>
-      <c r="C30" s="102" t="s">
+    <row r="30" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="123"/>
+      <c r="C30" s="121" t="s">
         <v>84</v>
       </c>
       <c r="D30" s="40" t="s">
@@ -3503,11 +3787,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
+      <c r="J30" s="102">
+        <v>0</v>
+      </c>
+      <c r="K30" s="102">
+        <v>0</v>
+      </c>
+      <c r="L30" s="102">
+        <v>0</v>
+      </c>
+      <c r="M30" s="102">
+        <v>0</v>
+      </c>
+      <c r="N30" s="102">
+        <v>0</v>
+      </c>
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
       <c r="Q30" s="32"/>
@@ -3532,9 +3826,9 @@
       <c r="AJ30" s="36"/>
       <c r="AK30" s="37"/>
     </row>
-    <row r="31" spans="2:37" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="104"/>
-      <c r="C31" s="102"/>
+    <row r="31" spans="2:37" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="123"/>
+      <c r="C31" s="121"/>
       <c r="D31" s="40" t="s">
         <v>55</v>
       </c>
@@ -3552,11 +3846,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
+      <c r="J31" s="102">
+        <v>0</v>
+      </c>
+      <c r="K31" s="102">
+        <v>0</v>
+      </c>
+      <c r="L31" s="102">
+        <v>0</v>
+      </c>
+      <c r="M31" s="102">
+        <v>0</v>
+      </c>
+      <c r="N31" s="102">
+        <v>0</v>
+      </c>
       <c r="O31" s="32"/>
       <c r="P31" s="32"/>
       <c r="Q31" s="32"/>
@@ -3581,9 +3885,9 @@
       <c r="AJ31" s="36"/>
       <c r="AK31" s="37"/>
     </row>
-    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="104"/>
-      <c r="C32" s="102"/>
+    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="123"/>
+      <c r="C32" s="121"/>
       <c r="D32" s="40" t="s">
         <v>48</v>
       </c>
@@ -3601,11 +3905,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
+      <c r="J32" s="102">
+        <v>0</v>
+      </c>
+      <c r="K32" s="102">
+        <v>0</v>
+      </c>
+      <c r="L32" s="102">
+        <v>0</v>
+      </c>
+      <c r="M32" s="102">
+        <v>0</v>
+      </c>
+      <c r="N32" s="102">
+        <v>0</v>
+      </c>
       <c r="O32" s="32"/>
       <c r="P32" s="32"/>
       <c r="Q32" s="32"/>
@@ -3630,8 +3944,8 @@
       <c r="AJ32" s="36"/>
       <c r="AK32" s="37"/>
     </row>
-    <row r="33" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="104"/>
+    <row r="33" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="123"/>
       <c r="C33" s="45" t="s">
         <v>59</v>
       </c>
@@ -3650,11 +3964,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
+      <c r="J33" s="102">
+        <v>0</v>
+      </c>
+      <c r="K33" s="102">
+        <v>0</v>
+      </c>
+      <c r="L33" s="102">
+        <v>0</v>
+      </c>
+      <c r="M33" s="102">
+        <v>0</v>
+      </c>
+      <c r="N33" s="102">
+        <v>0</v>
+      </c>
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="32"/>
@@ -3679,9 +4003,9 @@
       <c r="AJ33" s="36"/>
       <c r="AK33" s="37"/>
     </row>
-    <row r="34" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="104"/>
-      <c r="C34" s="118" t="s">
+    <row r="34" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="123"/>
+      <c r="C34" s="136" t="s">
         <v>77</v>
       </c>
       <c r="D34" s="41" t="s">
@@ -3701,11 +4025,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
+      <c r="J34" s="102">
+        <v>0</v>
+      </c>
+      <c r="K34" s="102">
+        <v>0</v>
+      </c>
+      <c r="L34" s="102">
+        <v>0</v>
+      </c>
+      <c r="M34" s="102">
+        <v>0</v>
+      </c>
+      <c r="N34" s="102">
+        <v>0</v>
+      </c>
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
       <c r="Q34" s="32"/>
@@ -3730,9 +4064,9 @@
       <c r="AJ34" s="36"/>
       <c r="AK34" s="37"/>
     </row>
-    <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="104"/>
-      <c r="C35" s="119"/>
+    <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="123"/>
+      <c r="C35" s="137"/>
       <c r="D35" s="40" t="s">
         <v>79</v>
       </c>
@@ -3750,11 +4084,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
+      <c r="J35" s="102">
+        <v>0</v>
+      </c>
+      <c r="K35" s="102">
+        <v>0</v>
+      </c>
+      <c r="L35" s="102">
+        <v>0</v>
+      </c>
+      <c r="M35" s="102">
+        <v>0</v>
+      </c>
+      <c r="N35" s="102">
+        <v>0</v>
+      </c>
       <c r="O35" s="32"/>
       <c r="P35" s="32"/>
       <c r="Q35" s="32"/>
@@ -3779,9 +4123,9 @@
       <c r="AJ35" s="36"/>
       <c r="AK35" s="37"/>
     </row>
-    <row r="36" spans="2:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="104"/>
-      <c r="C36" s="119"/>
+    <row r="36" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="123"/>
+      <c r="C36" s="137"/>
       <c r="D36" s="40" t="s">
         <v>82</v>
       </c>
@@ -3799,11 +4143,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
+      <c r="J36" s="102">
+        <v>0</v>
+      </c>
+      <c r="K36" s="102">
+        <v>0</v>
+      </c>
+      <c r="L36" s="102">
+        <v>0</v>
+      </c>
+      <c r="M36" s="102">
+        <v>0</v>
+      </c>
+      <c r="N36" s="102">
+        <v>0</v>
+      </c>
       <c r="O36" s="32"/>
       <c r="P36" s="32"/>
       <c r="Q36" s="32"/>
@@ -3828,9 +4182,9 @@
       <c r="AJ36" s="36"/>
       <c r="AK36" s="37"/>
     </row>
-    <row r="37" spans="2:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="104"/>
-      <c r="C37" s="119"/>
+    <row r="37" spans="2:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="123"/>
+      <c r="C37" s="137"/>
       <c r="D37" s="40" t="s">
         <v>81</v>
       </c>
@@ -3848,11 +4202,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="J37" s="102">
+        <v>0</v>
+      </c>
+      <c r="K37" s="102">
+        <v>0</v>
+      </c>
+      <c r="L37" s="102">
+        <v>0</v>
+      </c>
+      <c r="M37" s="102">
+        <v>0</v>
+      </c>
+      <c r="N37" s="102">
+        <v>0</v>
+      </c>
       <c r="O37" s="32"/>
       <c r="P37" s="32"/>
       <c r="Q37" s="32"/>
@@ -3877,9 +4241,9 @@
       <c r="AJ37" s="36"/>
       <c r="AK37" s="37"/>
     </row>
-    <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="104"/>
-      <c r="C38" s="120"/>
+    <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="123"/>
+      <c r="C38" s="138"/>
       <c r="D38" s="40" t="s">
         <v>80</v>
       </c>
@@ -3897,11 +4261,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
+      <c r="J38" s="102">
+        <v>0</v>
+      </c>
+      <c r="K38" s="102">
+        <v>0</v>
+      </c>
+      <c r="L38" s="102">
+        <v>0</v>
+      </c>
+      <c r="M38" s="102">
+        <v>0</v>
+      </c>
+      <c r="N38" s="102">
+        <v>0</v>
+      </c>
       <c r="O38" s="32"/>
       <c r="P38" s="32"/>
       <c r="Q38" s="32"/>
@@ -3926,9 +4300,9 @@
       <c r="AJ38" s="36"/>
       <c r="AK38" s="37"/>
     </row>
-    <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="104"/>
-      <c r="C39" s="109" t="s">
+    <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="123"/>
+      <c r="C39" s="128" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="40" t="s">
@@ -3948,11 +4322,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
+      <c r="J39" s="102">
+        <v>0</v>
+      </c>
+      <c r="K39" s="102">
+        <v>0</v>
+      </c>
+      <c r="L39" s="102">
+        <v>0</v>
+      </c>
+      <c r="M39" s="102">
+        <v>0</v>
+      </c>
+      <c r="N39" s="102">
+        <v>0</v>
+      </c>
       <c r="O39" s="32"/>
       <c r="P39" s="32"/>
       <c r="Q39" s="32"/>
@@ -3977,9 +4361,9 @@
       <c r="AJ39" s="36"/>
       <c r="AK39" s="37"/>
     </row>
-    <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="104"/>
-      <c r="C40" s="109"/>
+    <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="123"/>
+      <c r="C40" s="128"/>
       <c r="D40" s="40" t="s">
         <v>65</v>
       </c>
@@ -3997,11 +4381,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
+      <c r="J40" s="102">
+        <v>0</v>
+      </c>
+      <c r="K40" s="102">
+        <v>0</v>
+      </c>
+      <c r="L40" s="102">
+        <v>0</v>
+      </c>
+      <c r="M40" s="102">
+        <v>0</v>
+      </c>
+      <c r="N40" s="102">
+        <v>0</v>
+      </c>
       <c r="O40" s="32"/>
       <c r="P40" s="32"/>
       <c r="Q40" s="32"/>
@@ -4026,8 +4420,8 @@
       <c r="AJ40" s="36"/>
       <c r="AK40" s="37"/>
     </row>
-    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="104"/>
+    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="123"/>
       <c r="C41" s="44" t="s">
         <v>69</v>
       </c>
@@ -4046,11 +4440,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
+      <c r="J41" s="102">
+        <v>0</v>
+      </c>
+      <c r="K41" s="102">
+        <v>0</v>
+      </c>
+      <c r="L41" s="102">
+        <v>0</v>
+      </c>
+      <c r="M41" s="102">
+        <v>0</v>
+      </c>
+      <c r="N41" s="102">
+        <v>0</v>
+      </c>
       <c r="O41" s="32"/>
       <c r="P41" s="32"/>
       <c r="Q41" s="32"/>
@@ -4075,8 +4479,8 @@
       <c r="AJ41" s="36"/>
       <c r="AK41" s="37"/>
     </row>
-    <row r="42" spans="2:37" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="105"/>
+    <row r="42" spans="2:37" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="124"/>
       <c r="C42" s="78" t="s">
         <v>71</v>
       </c>
@@ -4095,11 +4499,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="55"/>
-      <c r="M42" s="55"/>
-      <c r="N42" s="55"/>
+      <c r="J42" s="140">
+        <v>0</v>
+      </c>
+      <c r="K42" s="140">
+        <v>0</v>
+      </c>
+      <c r="L42" s="140">
+        <v>0</v>
+      </c>
+      <c r="M42" s="140">
+        <v>0</v>
+      </c>
+      <c r="N42" s="140">
+        <v>0</v>
+      </c>
       <c r="O42" s="55"/>
       <c r="P42" s="55"/>
       <c r="Q42" s="55"/>
@@ -4124,8 +4538,8 @@
       <c r="AJ42" s="80"/>
       <c r="AK42" s="81"/>
     </row>
-    <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="110" t="s">
+    <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="129" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="82" t="s">
@@ -4146,11 +4560,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="29"/>
-      <c r="N43" s="29"/>
+      <c r="J43" s="139">
+        <v>0</v>
+      </c>
+      <c r="K43" s="139">
+        <v>0</v>
+      </c>
+      <c r="L43" s="139">
+        <v>0</v>
+      </c>
+      <c r="M43" s="139">
+        <v>0</v>
+      </c>
+      <c r="N43" s="139">
+        <v>0</v>
+      </c>
       <c r="O43" s="29"/>
       <c r="P43" s="29"/>
       <c r="Q43" s="29"/>
@@ -4175,8 +4599,8 @@
       <c r="AJ43" s="29"/>
       <c r="AK43" s="85"/>
     </row>
-    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="111"/>
+    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="130"/>
       <c r="C44" s="28" t="s">
         <v>27</v>
       </c>
@@ -4195,11 +4619,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
+      <c r="J44" s="102">
+        <v>0</v>
+      </c>
+      <c r="K44" s="102">
+        <v>0</v>
+      </c>
+      <c r="L44" s="102">
+        <v>0</v>
+      </c>
+      <c r="M44" s="102">
+        <v>0</v>
+      </c>
+      <c r="N44" s="102">
+        <v>0</v>
+      </c>
       <c r="O44" s="32"/>
       <c r="P44" s="32"/>
       <c r="Q44" s="32"/>
@@ -4224,9 +4658,9 @@
       <c r="AJ44" s="32"/>
       <c r="AK44" s="35"/>
     </row>
-    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="111"/>
-      <c r="C45" s="113" t="s">
+    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="130"/>
+      <c r="C45" s="132" t="s">
         <v>23</v>
       </c>
       <c r="D45" s="27" t="s">
@@ -4246,11 +4680,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
+      <c r="J45" s="102">
+        <v>0</v>
+      </c>
+      <c r="K45" s="102">
+        <v>0</v>
+      </c>
+      <c r="L45" s="102">
+        <v>0</v>
+      </c>
+      <c r="M45" s="102">
+        <v>0</v>
+      </c>
+      <c r="N45" s="102">
+        <v>0</v>
+      </c>
       <c r="O45" s="32"/>
       <c r="P45" s="32"/>
       <c r="Q45" s="32"/>
@@ -4275,9 +4719,9 @@
       <c r="AJ45" s="32"/>
       <c r="AK45" s="35"/>
     </row>
-    <row r="46" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="112"/>
-      <c r="C46" s="114"/>
+    <row r="46" spans="2:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="131"/>
+      <c r="C46" s="133"/>
       <c r="D46" s="52" t="s">
         <v>24</v>
       </c>
@@ -4295,11 +4739,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="55"/>
-      <c r="M46" s="55"/>
-      <c r="N46" s="55"/>
+      <c r="J46" s="140">
+        <v>0</v>
+      </c>
+      <c r="K46" s="140">
+        <v>0</v>
+      </c>
+      <c r="L46" s="140">
+        <v>0</v>
+      </c>
+      <c r="M46" s="140">
+        <v>0</v>
+      </c>
+      <c r="N46" s="140">
+        <v>0</v>
+      </c>
       <c r="O46" s="55"/>
       <c r="P46" s="55"/>
       <c r="Q46" s="55"/>
@@ -4324,8 +4778,8 @@
       <c r="AJ46" s="55"/>
       <c r="AK46" s="89"/>
     </row>
-    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="103" t="s">
+    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="122" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="90" t="s">
@@ -4346,11 +4800,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="29"/>
-      <c r="N47" s="29"/>
+      <c r="J47" s="139">
+        <v>0</v>
+      </c>
+      <c r="K47" s="139">
+        <v>0</v>
+      </c>
+      <c r="L47" s="139">
+        <v>0</v>
+      </c>
+      <c r="M47" s="139">
+        <v>0</v>
+      </c>
+      <c r="N47" s="139">
+        <v>0</v>
+      </c>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
@@ -4375,8 +4839,8 @@
       <c r="AJ47" s="29"/>
       <c r="AK47" s="85"/>
     </row>
-    <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="104"/>
+    <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="123"/>
       <c r="C48" s="42" t="s">
         <v>83</v>
       </c>
@@ -4393,14 +4857,26 @@
       </c>
       <c r="I48" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="J48" s="102">
+        <v>0</v>
+      </c>
+      <c r="K48" s="102">
+        <v>0</v>
+      </c>
+      <c r="L48" s="102">
+        <v>0</v>
+      </c>
+      <c r="M48" s="142">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="N48" s="142">
+        <v>0</v>
+      </c>
+      <c r="O48" s="106">
+        <v>0.05</v>
+      </c>
       <c r="P48" s="32"/>
       <c r="Q48" s="32"/>
       <c r="R48" s="32"/>
@@ -4424,8 +4900,8 @@
       <c r="AJ48" s="32"/>
       <c r="AK48" s="35"/>
     </row>
-    <row r="49" spans="2:37" ht="21" x14ac:dyDescent="0.25">
-      <c r="B49" s="104"/>
+    <row r="49" spans="2:37" ht="21" x14ac:dyDescent="0.3">
+      <c r="B49" s="123"/>
       <c r="C49" s="43" t="s">
         <v>67</v>
       </c>
@@ -4442,13 +4918,23 @@
       </c>
       <c r="I49" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="J49" s="102">
+        <v>0</v>
+      </c>
+      <c r="K49" s="102">
+        <v>0</v>
+      </c>
+      <c r="L49" s="142">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="M49" s="106">
+        <v>0.216</v>
+      </c>
+      <c r="N49" s="106">
+        <v>0</v>
+      </c>
       <c r="O49" s="36"/>
       <c r="P49" s="36"/>
       <c r="Q49" s="36"/>
@@ -4473,8 +4959,8 @@
       <c r="AJ49" s="36"/>
       <c r="AK49" s="37"/>
     </row>
-    <row r="50" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="105"/>
+    <row r="50" spans="2:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="124"/>
       <c r="C50" s="93" t="s">
         <v>68</v>
       </c>
@@ -4493,11 +4979,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-      <c r="L50" s="55"/>
-      <c r="M50" s="55"/>
-      <c r="N50" s="55"/>
+      <c r="J50" s="140">
+        <v>0</v>
+      </c>
+      <c r="K50" s="140">
+        <v>0</v>
+      </c>
+      <c r="L50" s="140">
+        <v>0</v>
+      </c>
+      <c r="M50" s="140">
+        <v>0</v>
+      </c>
+      <c r="N50" s="140">
+        <v>0</v>
+      </c>
       <c r="O50" s="80"/>
       <c r="P50" s="80"/>
       <c r="Q50" s="80"/>
@@ -4522,22 +5018,22 @@
       <c r="AJ50" s="80"/>
       <c r="AK50" s="81"/>
     </row>
-    <row r="51" spans="2:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="124" t="s">
+    <row r="51" spans="2:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="125"/>
-      <c r="D51" s="125"/>
-      <c r="E51" s="125"/>
-      <c r="F51" s="125"/>
-      <c r="G51" s="125"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="116"/>
       <c r="H51" s="13">
         <f t="shared" ref="H51:AK51" si="1">SUM(H4:H50)</f>
         <v>32.299999999999997</v>
       </c>
       <c r="I51" s="13">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.76429999999999998</v>
       </c>
       <c r="J51" s="13">
         <f t="shared" si="1"/>
@@ -4545,15 +5041,15 @@
       </c>
       <c r="K51" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.9299999999999999E-2</v>
       </c>
       <c r="L51" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="M51" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.249</v>
       </c>
       <c r="N51" s="13">
         <f t="shared" si="1"/>
@@ -4561,7 +5057,7 @@
       </c>
       <c r="O51" s="13">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="P51" s="13">
         <f t="shared" si="1"/>
@@ -4652,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4661,38 +5157,38 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="96" t="s">
+      <c r="J52" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="K52" s="97"/>
-      <c r="L52" s="97"/>
-      <c r="M52" s="97"/>
-      <c r="N52" s="97"/>
-      <c r="O52" s="97"/>
-      <c r="P52" s="97"/>
-      <c r="Q52" s="97"/>
-      <c r="R52" s="97"/>
-      <c r="S52" s="97"/>
-      <c r="T52" s="97"/>
-      <c r="U52" s="97"/>
-      <c r="V52" s="97"/>
-      <c r="W52" s="97"/>
-      <c r="X52" s="97"/>
-      <c r="Y52" s="97"/>
-      <c r="Z52" s="97"/>
-      <c r="AA52" s="97"/>
-      <c r="AB52" s="97"/>
-      <c r="AC52" s="97"/>
-      <c r="AD52" s="97"/>
-      <c r="AE52" s="97"/>
-      <c r="AF52" s="97"/>
-      <c r="AG52" s="97"/>
-      <c r="AH52" s="97"/>
-      <c r="AI52" s="97"/>
-      <c r="AJ52" s="97"/>
-      <c r="AK52" s="98"/>
-    </row>
-    <row r="53" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K52" s="111"/>
+      <c r="L52" s="111"/>
+      <c r="M52" s="111"/>
+      <c r="N52" s="111"/>
+      <c r="O52" s="111"/>
+      <c r="P52" s="111"/>
+      <c r="Q52" s="111"/>
+      <c r="R52" s="111"/>
+      <c r="S52" s="111"/>
+      <c r="T52" s="111"/>
+      <c r="U52" s="111"/>
+      <c r="V52" s="111"/>
+      <c r="W52" s="111"/>
+      <c r="X52" s="111"/>
+      <c r="Y52" s="111"/>
+      <c r="Z52" s="111"/>
+      <c r="AA52" s="111"/>
+      <c r="AB52" s="111"/>
+      <c r="AC52" s="111"/>
+      <c r="AD52" s="111"/>
+      <c r="AE52" s="111"/>
+      <c r="AF52" s="111"/>
+      <c r="AG52" s="111"/>
+      <c r="AH52" s="111"/>
+      <c r="AI52" s="111"/>
+      <c r="AJ52" s="111"/>
+      <c r="AK52" s="117"/>
+    </row>
+    <row r="53" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="19" t="s">
         <v>31</v>
       </c>
@@ -4716,7 +5212,7 @@
       <c r="O53" s="8"/>
       <c r="P53" s="8"/>
     </row>
-    <row r="54" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="25" t="s">
         <v>16</v>
       </c>
@@ -4728,130 +5224,130 @@
         <f>SUM(I4:I9,I14,I15,I18,I43:I46)</f>
         <v>0</v>
       </c>
-      <c r="E54" s="127">
+      <c r="E54" s="97">
         <f>SUM(C54,-D55)</f>
-        <v>10.65</v>
+        <v>10.1357</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="96" t="s">
+      <c r="H54" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="I54" s="121"/>
+      <c r="I54" s="110"/>
       <c r="J54" s="9">
         <f>H51-J51</f>
         <v>32.299999999999997</v>
       </c>
       <c r="K54" s="9">
         <f>J54-K51</f>
-        <v>32.299999999999997</v>
+        <v>32.200699999999998</v>
       </c>
       <c r="L54" s="9">
         <f>K54-L51</f>
-        <v>32.299999999999997</v>
+        <v>32.084699999999998</v>
       </c>
       <c r="M54" s="9">
         <f>L54-M51</f>
-        <v>32.299999999999997</v>
+        <v>31.835699999999999</v>
       </c>
       <c r="N54" s="9">
         <f t="shared" ref="N54:W54" si="2">M54-N51</f>
-        <v>32.299999999999997</v>
+        <v>31.835699999999999</v>
       </c>
       <c r="O54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="P54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="Q54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="R54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="S54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="T54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="U54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="V54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="W54" s="9">
         <f t="shared" si="2"/>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="X54" s="9">
         <f t="shared" ref="X54" si="3">W54-X51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="Y54" s="9">
         <f t="shared" ref="Y54" si="4">X54-Y51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="Z54" s="9">
         <f t="shared" ref="Z54" si="5">Y54-Z51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AA54" s="9">
         <f t="shared" ref="AA54" si="6">Z54-AA51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AB54" s="9">
         <f t="shared" ref="AB54" si="7">AA54-AB51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AC54" s="9">
         <f t="shared" ref="AC54" si="8">AB54-AC51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AD54" s="9">
         <f t="shared" ref="AD54" si="9">AC54-AD51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AE54" s="9">
         <f t="shared" ref="AE54" si="10">AD54-AE51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AF54" s="9">
         <f t="shared" ref="AF54" si="11">AE54-AF51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AG54" s="9">
         <f t="shared" ref="AG54" si="12">AF54-AG51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AH54" s="9">
         <f t="shared" ref="AH54" si="13">AG54-AH51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AI54" s="9">
         <f t="shared" ref="AI54" si="14">AH54-AI51</f>
-        <v>32.049999999999997</v>
+        <v>31.535699999999999</v>
       </c>
       <c r="AJ54" s="9">
         <f t="shared" ref="AJ54" si="15">AI54-AJ51</f>
-        <v>32.049999999999997</v>
-      </c>
-      <c r="AK54" s="126">
+        <v>31.535699999999999</v>
+      </c>
+      <c r="AK54" s="96">
         <f t="shared" ref="AK54" si="16">AJ54-AK51</f>
-        <v>32.049999999999997</v>
-      </c>
-    </row>
-    <row r="55" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31.535699999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="23" t="s">
         <v>15</v>
       </c>
@@ -4861,9 +5357,9 @@
       </c>
       <c r="D55" s="95">
         <f>SUM(I13,I16,I17,I19:I22,I24:I29,I34,I33,I41,I47:I50)</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="127">
+        <v>0.51429999999999998</v>
+      </c>
+      <c r="E55" s="97">
         <f t="shared" ref="E55:E56" si="17">SUM(C55,-D56)</f>
         <v>9.5500000000000007</v>
       </c>
@@ -4876,60 +5372,60 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="128">
+      <c r="C56" s="98">
         <f>SUM(H42,H35:H40,H30:H32,H23,H10:H12)</f>
         <v>11.85</v>
       </c>
-      <c r="D56" s="129">
+      <c r="D56" s="99">
         <f>SUM(I10:I12,I23,I30:I32,I35:I40,I42)</f>
         <v>0.25</v>
       </c>
-      <c r="E56" s="130">
+      <c r="E56" s="100">
         <f t="shared" si="17"/>
         <v>11.85</v>
       </c>
       <c r="F56" s="3"/>
-      <c r="H56" s="96" t="s">
+      <c r="H56" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="I56" s="97"/>
-      <c r="J56" s="96">
+      <c r="I56" s="111"/>
+      <c r="J56" s="109">
         <f>H51-I51</f>
-        <v>32.049999999999997</v>
-      </c>
-      <c r="K56" s="97"/>
-      <c r="L56" s="97"/>
-      <c r="M56" s="97"/>
-      <c r="N56" s="97"/>
-      <c r="O56" s="97"/>
-      <c r="P56" s="97"/>
-      <c r="Q56" s="97"/>
-      <c r="R56" s="97"/>
-      <c r="S56" s="97"/>
-      <c r="T56" s="97"/>
-      <c r="U56" s="97"/>
-      <c r="V56" s="97"/>
-      <c r="W56" s="97"/>
-      <c r="X56" s="97"/>
-      <c r="Y56" s="97"/>
-      <c r="Z56" s="97"/>
-      <c r="AA56" s="97"/>
-      <c r="AB56" s="97"/>
-      <c r="AC56" s="97"/>
-      <c r="AD56" s="97"/>
-      <c r="AE56" s="97"/>
-      <c r="AF56" s="97"/>
-      <c r="AG56" s="97"/>
-      <c r="AH56" s="97"/>
-      <c r="AI56" s="97"/>
-      <c r="AJ56" s="97"/>
-      <c r="AK56" s="98"/>
-    </row>
-    <row r="57" spans="2:37" x14ac:dyDescent="0.25">
+        <v>31.535699999999999</v>
+      </c>
+      <c r="K56" s="111"/>
+      <c r="L56" s="111"/>
+      <c r="M56" s="111"/>
+      <c r="N56" s="111"/>
+      <c r="O56" s="111"/>
+      <c r="P56" s="111"/>
+      <c r="Q56" s="111"/>
+      <c r="R56" s="111"/>
+      <c r="S56" s="111"/>
+      <c r="T56" s="111"/>
+      <c r="U56" s="111"/>
+      <c r="V56" s="111"/>
+      <c r="W56" s="111"/>
+      <c r="X56" s="111"/>
+      <c r="Y56" s="111"/>
+      <c r="Z56" s="111"/>
+      <c r="AA56" s="111"/>
+      <c r="AB56" s="111"/>
+      <c r="AC56" s="111"/>
+      <c r="AD56" s="111"/>
+      <c r="AE56" s="111"/>
+      <c r="AF56" s="111"/>
+      <c r="AG56" s="111"/>
+      <c r="AH56" s="111"/>
+      <c r="AI56" s="111"/>
+      <c r="AJ56" s="111"/>
+      <c r="AK56" s="117"/>
+    </row>
+    <row r="57" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -4943,7 +5439,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -4957,7 +5453,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -4971,48 +5467,42 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="J56:AK56"/>
-    <mergeCell ref="J52:AK52"/>
     <mergeCell ref="J2:AK2"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="C19:C29"/>
@@ -5025,6 +5515,12 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C34:C38"/>
     <mergeCell ref="B14:B42"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="J56:AK56"/>
+    <mergeCell ref="J52:AK52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5038,7 +5534,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5050,7 +5546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado excel y empezando a hacer el .js de la sala secreta de la dungeon
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
@@ -962,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1320,31 +1320,19 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1398,6 +1386,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1416,13 +1410,22 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1627,46 +1630,46 @@
                   <c:v>18.378999999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18.378999999999994</c:v>
+                  <c:v>16.698999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2111,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK16" sqref="AK16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AK36" sqref="AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,36 +2144,36 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="123" t="s">
+      <c r="J2" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="125"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
-      <c r="AC2" s="125"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="125"/>
-      <c r="AF2" s="125"/>
-      <c r="AG2" s="125"/>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="125"/>
-      <c r="AJ2" s="125"/>
-      <c r="AK2" s="132"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="127"/>
+      <c r="W2" s="127"/>
+      <c r="X2" s="127"/>
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="128"/>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
@@ -2283,7 +2286,7 @@
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="154" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="33" t="s">
@@ -2392,7 +2395,7 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="127"/>
+      <c r="B5" s="145"/>
       <c r="C5" s="102" t="s">
         <v>85</v>
       </c>
@@ -2499,7 +2502,7 @@
       </c>
     </row>
     <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="128"/>
+      <c r="B6" s="146"/>
       <c r="C6" s="27" t="s">
         <v>73</v>
       </c>
@@ -2606,7 +2609,7 @@
       </c>
     </row>
     <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="128"/>
+      <c r="B7" s="146"/>
       <c r="C7" s="27" t="s">
         <v>37</v>
       </c>
@@ -2713,7 +2716,7 @@
       </c>
     </row>
     <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="128"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="27" t="s">
         <v>39</v>
       </c>
@@ -2818,7 +2821,7 @@
       </c>
     </row>
     <row r="9" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="129"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="47" t="s">
         <v>40</v>
       </c>
@@ -2925,7 +2928,7 @@
       </c>
     </row>
     <row r="10" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="153" t="s">
+      <c r="B10" s="151" t="s">
         <v>86</v>
       </c>
       <c r="C10" s="107" t="s">
@@ -3034,7 +3037,7 @@
       </c>
     </row>
     <row r="11" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="154"/>
+      <c r="B11" s="152"/>
       <c r="C11" s="114" t="s">
         <v>87</v>
       </c>
@@ -3250,10 +3253,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="145" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="136" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="52" t="s">
@@ -3361,8 +3364,8 @@
       </c>
     </row>
     <row r="14" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="128"/>
-      <c r="C14" s="141"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="137"/>
       <c r="D14" s="35" t="s">
         <v>60</v>
       </c>
@@ -3468,8 +3471,8 @@
       </c>
     </row>
     <row r="15" spans="1:37" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="149"/>
-      <c r="C15" s="142"/>
+      <c r="B15" s="147"/>
+      <c r="C15" s="138"/>
       <c r="D15" s="58" t="s">
         <v>61</v>
       </c>
@@ -3519,58 +3522,58 @@
       <c r="S15" s="96">
         <v>0</v>
       </c>
-      <c r="T15" s="156">
+      <c r="T15" s="124">
         <v>0.83</v>
       </c>
-      <c r="U15" s="156">
-        <v>0</v>
-      </c>
-      <c r="V15" s="156">
-        <v>0</v>
-      </c>
-      <c r="W15" s="156">
-        <v>0</v>
-      </c>
-      <c r="X15" s="156">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="156">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AI15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="156">
-        <v>0</v>
-      </c>
-      <c r="AK15" s="157">
+      <c r="U15" s="124">
+        <v>0</v>
+      </c>
+      <c r="V15" s="124">
+        <v>0</v>
+      </c>
+      <c r="W15" s="124">
+        <v>0</v>
+      </c>
+      <c r="X15" s="124">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="124">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="124">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="125">
         <v>0</v>
       </c>
     </row>
@@ -3648,10 +3651,10 @@
       <c r="AK16" s="57"/>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="137" t="s">
+      <c r="B17" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="129" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="66" t="s">
@@ -3757,8 +3760,8 @@
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="138"/>
-      <c r="C18" s="134"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="27" t="s">
         <v>75</v>
       </c>
@@ -3862,8 +3865,8 @@
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="138"/>
-      <c r="C19" s="134"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="36" t="s">
         <v>50</v>
       </c>
@@ -3914,27 +3917,61 @@
       <c r="T19" s="116">
         <v>0.83</v>
       </c>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="30"/>
-      <c r="Z19" s="30"/>
-      <c r="AA19" s="30"/>
-      <c r="AB19" s="30"/>
-      <c r="AC19" s="30"/>
-      <c r="AD19" s="30"/>
-      <c r="AE19" s="30"/>
-      <c r="AF19" s="30"/>
-      <c r="AG19" s="30"/>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="31"/>
-      <c r="AJ19" s="31"/>
-      <c r="AK19" s="32"/>
+      <c r="U19" s="94">
+        <v>0</v>
+      </c>
+      <c r="V19" s="94">
+        <v>0</v>
+      </c>
+      <c r="W19" s="94">
+        <v>0</v>
+      </c>
+      <c r="X19" s="94">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="94">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="94">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="138"/>
-      <c r="C20" s="134"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="130"/>
       <c r="D20" s="36" t="s">
         <v>33</v>
       </c>
@@ -3985,27 +4022,61 @@
       <c r="T20" s="116">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="30"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="30"/>
-      <c r="AA20" s="30"/>
-      <c r="AB20" s="30"/>
-      <c r="AC20" s="30"/>
-      <c r="AD20" s="30"/>
-      <c r="AE20" s="30"/>
-      <c r="AF20" s="30"/>
-      <c r="AG20" s="30"/>
-      <c r="AH20" s="31"/>
-      <c r="AI20" s="31"/>
-      <c r="AJ20" s="31"/>
-      <c r="AK20" s="32"/>
+      <c r="U20" s="94">
+        <v>0</v>
+      </c>
+      <c r="V20" s="94">
+        <v>0</v>
+      </c>
+      <c r="W20" s="94">
+        <v>0</v>
+      </c>
+      <c r="X20" s="94">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="94">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="94">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="138"/>
-      <c r="C21" s="134"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="130"/>
       <c r="D21" s="27" t="s">
         <v>34</v>
       </c>
@@ -4070,11 +4141,11 @@
       <c r="AH21" s="31"/>
       <c r="AI21" s="31"/>
       <c r="AJ21" s="31"/>
-      <c r="AK21" s="32"/>
+      <c r="AK21" s="158"/>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="138"/>
-      <c r="C22" s="135" t="s">
+      <c r="B22" s="134"/>
+      <c r="C22" s="131" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="36" t="s">
@@ -4127,27 +4198,61 @@
       <c r="T22" s="116">
         <v>1.6E-2</v>
       </c>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="30"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="30"/>
-      <c r="AD22" s="30"/>
-      <c r="AE22" s="30"/>
-      <c r="AF22" s="30"/>
-      <c r="AG22" s="30"/>
-      <c r="AH22" s="31"/>
-      <c r="AI22" s="31"/>
-      <c r="AJ22" s="31"/>
-      <c r="AK22" s="32"/>
+      <c r="U22" s="116">
+        <v>0</v>
+      </c>
+      <c r="V22" s="116">
+        <v>0</v>
+      </c>
+      <c r="W22" s="116">
+        <v>0</v>
+      </c>
+      <c r="X22" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="138"/>
-      <c r="C23" s="135"/>
+      <c r="B23" s="134"/>
+      <c r="C23" s="131"/>
       <c r="D23" s="36" t="s">
         <v>45</v>
       </c>
@@ -4198,27 +4303,61 @@
       <c r="T23" s="116">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="30"/>
-      <c r="Y23" s="30"/>
-      <c r="Z23" s="30"/>
-      <c r="AA23" s="30"/>
-      <c r="AB23" s="30"/>
-      <c r="AC23" s="30"/>
-      <c r="AD23" s="30"/>
-      <c r="AE23" s="30"/>
-      <c r="AF23" s="30"/>
-      <c r="AG23" s="30"/>
-      <c r="AH23" s="31"/>
-      <c r="AI23" s="31"/>
-      <c r="AJ23" s="31"/>
-      <c r="AK23" s="32"/>
+      <c r="U23" s="116">
+        <v>0</v>
+      </c>
+      <c r="V23" s="116">
+        <v>0</v>
+      </c>
+      <c r="W23" s="116">
+        <v>0</v>
+      </c>
+      <c r="X23" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="138"/>
-      <c r="C24" s="135"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="131"/>
       <c r="D24" s="36" t="s">
         <v>46</v>
       </c>
@@ -4269,27 +4408,61 @@
       <c r="T24" s="116">
         <v>0.11600000000000001</v>
       </c>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30"/>
-      <c r="AA24" s="30"/>
-      <c r="AB24" s="30"/>
-      <c r="AC24" s="30"/>
-      <c r="AD24" s="30"/>
-      <c r="AE24" s="30"/>
-      <c r="AF24" s="30"/>
-      <c r="AG24" s="30"/>
-      <c r="AH24" s="31"/>
-      <c r="AI24" s="31"/>
-      <c r="AJ24" s="31"/>
-      <c r="AK24" s="32"/>
+      <c r="U24" s="116">
+        <v>0</v>
+      </c>
+      <c r="V24" s="116">
+        <v>0</v>
+      </c>
+      <c r="W24" s="116">
+        <v>0</v>
+      </c>
+      <c r="X24" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="138"/>
-      <c r="C25" s="135"/>
+      <c r="B25" s="134"/>
+      <c r="C25" s="131"/>
       <c r="D25" s="36" t="s">
         <v>47</v>
       </c>
@@ -4340,27 +4513,61 @@
       <c r="T25" s="117">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="U25" s="31"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="30"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="30"/>
-      <c r="AG25" s="30"/>
-      <c r="AH25" s="31"/>
-      <c r="AI25" s="31"/>
-      <c r="AJ25" s="31"/>
-      <c r="AK25" s="32"/>
+      <c r="U25" s="116">
+        <v>0</v>
+      </c>
+      <c r="V25" s="116">
+        <v>0</v>
+      </c>
+      <c r="W25" s="116">
+        <v>0</v>
+      </c>
+      <c r="X25" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="94">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="138"/>
-      <c r="C26" s="135"/>
+      <c r="B26" s="134"/>
+      <c r="C26" s="131"/>
       <c r="D26" s="35" t="s">
         <v>48</v>
       </c>
@@ -4428,8 +4635,8 @@
       <c r="AK26" s="32"/>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="138"/>
-      <c r="C27" s="135"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="131"/>
       <c r="D27" s="36" t="s">
         <v>51</v>
       </c>
@@ -4480,27 +4687,61 @@
       <c r="T27" s="117">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="31"/>
-      <c r="AI27" s="31"/>
-      <c r="AJ27" s="31"/>
-      <c r="AK27" s="32"/>
+      <c r="U27" s="116">
+        <v>0</v>
+      </c>
+      <c r="V27" s="116">
+        <v>0</v>
+      </c>
+      <c r="W27" s="116">
+        <v>0</v>
+      </c>
+      <c r="X27" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="138"/>
-      <c r="C28" s="135"/>
+      <c r="B28" s="134"/>
+      <c r="C28" s="131"/>
       <c r="D28" s="36" t="s">
         <v>52</v>
       </c>
@@ -4551,27 +4792,61 @@
       <c r="T28" s="116">
         <v>0.1</v>
       </c>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="30"/>
-      <c r="AD28" s="30"/>
-      <c r="AE28" s="30"/>
-      <c r="AF28" s="30"/>
-      <c r="AG28" s="30"/>
-      <c r="AH28" s="31"/>
-      <c r="AI28" s="31"/>
-      <c r="AJ28" s="31"/>
-      <c r="AK28" s="32"/>
+      <c r="U28" s="116">
+        <v>0</v>
+      </c>
+      <c r="V28" s="116">
+        <v>0</v>
+      </c>
+      <c r="W28" s="116">
+        <v>0</v>
+      </c>
+      <c r="X28" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="138"/>
-      <c r="C29" s="135"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="131"/>
       <c r="D29" s="36" t="s">
         <v>53</v>
       </c>
@@ -4622,27 +4897,61 @@
       <c r="T29" s="116">
         <v>0.35</v>
       </c>
-      <c r="U29" s="31"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="31"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="30"/>
-      <c r="AB29" s="30"/>
-      <c r="AC29" s="30"/>
-      <c r="AD29" s="30"/>
-      <c r="AE29" s="30"/>
-      <c r="AF29" s="30"/>
-      <c r="AG29" s="30"/>
-      <c r="AH29" s="31"/>
-      <c r="AI29" s="31"/>
-      <c r="AJ29" s="31"/>
-      <c r="AK29" s="32"/>
+      <c r="U29" s="116">
+        <v>0</v>
+      </c>
+      <c r="V29" s="116">
+        <v>0</v>
+      </c>
+      <c r="W29" s="116">
+        <v>0</v>
+      </c>
+      <c r="X29" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="138"/>
-      <c r="C30" s="135"/>
+      <c r="B30" s="134"/>
+      <c r="C30" s="131"/>
       <c r="D30" s="36" t="s">
         <v>57</v>
       </c>
@@ -4693,27 +5002,61 @@
       <c r="T30" s="94">
         <v>1.6E-2</v>
       </c>
-      <c r="U30" s="31"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="30"/>
-      <c r="AC30" s="30"/>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30"/>
-      <c r="AF30" s="30"/>
-      <c r="AG30" s="30"/>
-      <c r="AH30" s="31"/>
-      <c r="AI30" s="31"/>
-      <c r="AJ30" s="31"/>
-      <c r="AK30" s="32"/>
+      <c r="U30" s="116">
+        <v>0</v>
+      </c>
+      <c r="V30" s="116">
+        <v>0</v>
+      </c>
+      <c r="W30" s="116">
+        <v>0</v>
+      </c>
+      <c r="X30" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="138"/>
-      <c r="C31" s="135"/>
+      <c r="B31" s="134"/>
+      <c r="C31" s="131"/>
       <c r="D31" s="36" t="s">
         <v>55</v>
       </c>
@@ -4764,27 +5107,61 @@
       <c r="T31" s="116">
         <v>0.28299999999999997</v>
       </c>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="31"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="30"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="30"/>
-      <c r="AE31" s="30"/>
-      <c r="AF31" s="30"/>
-      <c r="AG31" s="30"/>
-      <c r="AH31" s="31"/>
-      <c r="AI31" s="31"/>
-      <c r="AJ31" s="31"/>
-      <c r="AK31" s="32"/>
+      <c r="U31" s="116">
+        <v>0</v>
+      </c>
+      <c r="V31" s="116">
+        <v>0</v>
+      </c>
+      <c r="W31" s="116">
+        <v>0</v>
+      </c>
+      <c r="X31" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ31" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="138"/>
-      <c r="C32" s="135"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="131"/>
       <c r="D32" s="36" t="s">
         <v>56</v>
       </c>
@@ -4835,27 +5212,61 @@
       <c r="T32" s="116">
         <v>0.05</v>
       </c>
-      <c r="U32" s="31"/>
-      <c r="V32" s="31"/>
-      <c r="W32" s="31"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="30"/>
-      <c r="AE32" s="30"/>
-      <c r="AF32" s="30"/>
-      <c r="AG32" s="30"/>
-      <c r="AH32" s="31"/>
-      <c r="AI32" s="31"/>
-      <c r="AJ32" s="31"/>
-      <c r="AK32" s="32"/>
+      <c r="U32" s="116">
+        <v>0</v>
+      </c>
+      <c r="V32" s="116">
+        <v>0</v>
+      </c>
+      <c r="W32" s="116">
+        <v>0</v>
+      </c>
+      <c r="X32" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="138"/>
-      <c r="C33" s="136" t="s">
+      <c r="B33" s="134"/>
+      <c r="C33" s="132" t="s">
         <v>83</v>
       </c>
       <c r="D33" s="35" t="s">
@@ -4956,13 +5367,13 @@
       <c r="AJ33" s="94">
         <v>0</v>
       </c>
-      <c r="AK33" s="155">
+      <c r="AK33" s="123">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:37" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="138"/>
-      <c r="C34" s="136"/>
+      <c r="B34" s="134"/>
+      <c r="C34" s="132"/>
       <c r="D34" s="35" t="s">
         <v>54</v>
       </c>
@@ -5030,7 +5441,7 @@
       <c r="AK34" s="32"/>
     </row>
     <row r="35" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="138"/>
+      <c r="B35" s="134"/>
       <c r="C35" s="40" t="s">
         <v>58</v>
       </c>
@@ -5082,27 +5493,61 @@
       <c r="T35" s="116">
         <v>0.15</v>
       </c>
-      <c r="U35" s="31"/>
-      <c r="V35" s="31"/>
-      <c r="W35" s="31"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-      <c r="AC35" s="30"/>
-      <c r="AD35" s="30"/>
-      <c r="AE35" s="30"/>
-      <c r="AF35" s="30"/>
-      <c r="AG35" s="30"/>
-      <c r="AH35" s="31"/>
-      <c r="AI35" s="31"/>
-      <c r="AJ35" s="31"/>
-      <c r="AK35" s="32"/>
+      <c r="U35" s="116">
+        <v>0</v>
+      </c>
+      <c r="V35" s="116">
+        <v>0</v>
+      </c>
+      <c r="W35" s="116">
+        <v>0</v>
+      </c>
+      <c r="X35" s="116">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="116">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="116">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="138"/>
-      <c r="C36" s="150" t="s">
+      <c r="B36" s="134"/>
+      <c r="C36" s="148" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="36" t="s">
@@ -5174,8 +5619,8 @@
       <c r="AK36" s="32"/>
     </row>
     <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="138"/>
-      <c r="C37" s="151"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="149"/>
       <c r="D37" s="35" t="s">
         <v>78</v>
       </c>
@@ -5243,8 +5688,8 @@
       <c r="AK37" s="32"/>
     </row>
     <row r="38" spans="2:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="138"/>
-      <c r="C38" s="151"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="149"/>
       <c r="D38" s="35" t="s">
         <v>81</v>
       </c>
@@ -5312,8 +5757,8 @@
       <c r="AK38" s="32"/>
     </row>
     <row r="39" spans="2:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="138"/>
-      <c r="C39" s="151"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="149"/>
       <c r="D39" s="35" t="s">
         <v>80</v>
       </c>
@@ -5361,28 +5806,64 @@
       <c r="S39" s="91">
         <v>0</v>
       </c>
-      <c r="T39" s="31"/>
-      <c r="U39" s="31"/>
-      <c r="V39" s="31"/>
-      <c r="W39" s="31"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
-      <c r="AF39" s="30"/>
-      <c r="AG39" s="30"/>
-      <c r="AH39" s="31"/>
-      <c r="AI39" s="31"/>
-      <c r="AJ39" s="31"/>
-      <c r="AK39" s="32"/>
+      <c r="T39" s="91">
+        <v>0</v>
+      </c>
+      <c r="U39" s="91">
+        <v>0</v>
+      </c>
+      <c r="V39" s="91">
+        <v>0</v>
+      </c>
+      <c r="W39" s="91">
+        <v>0</v>
+      </c>
+      <c r="X39" s="94">
+        <v>1.3</v>
+      </c>
+      <c r="Y39" s="94">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="94">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="138"/>
-      <c r="C40" s="152"/>
+      <c r="B40" s="134"/>
+      <c r="C40" s="150"/>
       <c r="D40" s="35" t="s">
         <v>79</v>
       </c>
@@ -5430,28 +5911,64 @@
       <c r="S40" s="91">
         <v>0</v>
       </c>
-      <c r="T40" s="31"/>
-      <c r="U40" s="31"/>
-      <c r="V40" s="31"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="30"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="30"/>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AE40" s="30"/>
-      <c r="AF40" s="30"/>
-      <c r="AG40" s="30"/>
-      <c r="AH40" s="31"/>
-      <c r="AI40" s="31"/>
-      <c r="AJ40" s="31"/>
-      <c r="AK40" s="32"/>
+      <c r="T40" s="91">
+        <v>0</v>
+      </c>
+      <c r="U40" s="91">
+        <v>0</v>
+      </c>
+      <c r="V40" s="91">
+        <v>0</v>
+      </c>
+      <c r="W40" s="91">
+        <v>0</v>
+      </c>
+      <c r="X40" s="94">
+        <v>0.38</v>
+      </c>
+      <c r="Y40" s="94">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="94">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="138"/>
-      <c r="C41" s="143" t="s">
+      <c r="B41" s="134"/>
+      <c r="C41" s="139" t="s">
         <v>62</v>
       </c>
       <c r="D41" s="35" t="s">
@@ -5521,8 +6038,8 @@
       <c r="AK41" s="32"/>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="138"/>
-      <c r="C42" s="143"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="139"/>
       <c r="D42" s="35" t="s">
         <v>64</v>
       </c>
@@ -5590,7 +6107,7 @@
       <c r="AK42" s="32"/>
     </row>
     <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="138"/>
+      <c r="B43" s="134"/>
       <c r="C43" s="39" t="s">
         <v>68</v>
       </c>
@@ -5642,26 +6159,60 @@
       <c r="T43" s="94">
         <v>0</v>
       </c>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="30"/>
-      <c r="Y43" s="30"/>
-      <c r="Z43" s="30"/>
-      <c r="AA43" s="30"/>
-      <c r="AB43" s="30"/>
-      <c r="AC43" s="30"/>
-      <c r="AD43" s="30"/>
-      <c r="AE43" s="30"/>
-      <c r="AF43" s="30"/>
-      <c r="AG43" s="30"/>
-      <c r="AH43" s="31"/>
-      <c r="AI43" s="31"/>
-      <c r="AJ43" s="31"/>
-      <c r="AK43" s="32"/>
+      <c r="U43" s="94">
+        <v>0</v>
+      </c>
+      <c r="V43" s="94">
+        <v>0</v>
+      </c>
+      <c r="W43" s="94">
+        <v>0</v>
+      </c>
+      <c r="X43" s="94">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="94">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="94">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="123">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="2:37" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="139"/>
+      <c r="B44" s="135"/>
       <c r="C44" s="67" t="s">
         <v>70</v>
       </c>
@@ -5730,7 +6281,7 @@
       <c r="AK44" s="70"/>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="144" t="s">
+      <c r="B45" s="140" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="71" t="s">
@@ -5837,7 +6388,7 @@
       </c>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="145"/>
+      <c r="B46" s="141"/>
       <c r="C46" s="28" t="s">
         <v>27</v>
       </c>
@@ -5942,8 +6493,8 @@
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="145"/>
-      <c r="C47" s="147" t="s">
+      <c r="B47" s="141"/>
+      <c r="C47" s="143" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="27" t="s">
@@ -6049,8 +6600,8 @@
       </c>
     </row>
     <row r="48" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="146"/>
-      <c r="C48" s="148"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="144"/>
       <c r="D48" s="47" t="s">
         <v>24</v>
       </c>
@@ -6124,7 +6675,7 @@
       <c r="AK48" s="78"/>
     </row>
     <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="133" t="s">
         <v>14</v>
       </c>
       <c r="C49" s="79" t="s">
@@ -6197,7 +6748,7 @@
       <c r="AK49" s="74"/>
     </row>
     <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="138"/>
+      <c r="B50" s="134"/>
       <c r="C50" s="37" t="s">
         <v>82</v>
       </c>
@@ -6302,7 +6853,7 @@
       </c>
     </row>
     <row r="51" spans="2:37" ht="21" x14ac:dyDescent="0.25">
-      <c r="B51" s="138"/>
+      <c r="B51" s="134"/>
       <c r="C51" s="38" t="s">
         <v>66</v>
       </c>
@@ -6407,7 +6958,7 @@
       </c>
     </row>
     <row r="52" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="139"/>
+      <c r="B52" s="135"/>
       <c r="C52" s="82" t="s">
         <v>67</v>
       </c>
@@ -6512,132 +7063,132 @@
       </c>
     </row>
     <row r="53" spans="2:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="130" t="s">
+      <c r="B53" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="131"/>
+      <c r="C53" s="157"/>
+      <c r="D53" s="157"/>
+      <c r="E53" s="157"/>
+      <c r="F53" s="157"/>
+      <c r="G53" s="157"/>
       <c r="H53" s="13">
-        <f>SUM(H4:H52)</f>
+        <f t="shared" ref="H53:AK53" si="1">SUM(H4:H52)</f>
         <v>30.199999999999996</v>
       </c>
       <c r="I53" s="13">
-        <f>SUM(I4:I52)</f>
+        <f t="shared" si="1"/>
         <v>11.821000000000003</v>
       </c>
       <c r="J53" s="13">
-        <f>SUM(J4:J52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" s="13">
-        <f>SUM(K4:K52)</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="L53" s="13">
-        <f>SUM(L4:L52)</f>
+        <f t="shared" si="1"/>
         <v>0.11600000000000001</v>
       </c>
       <c r="M53" s="13">
-        <f>SUM(M4:M52)</f>
+        <f t="shared" si="1"/>
         <v>0.249</v>
       </c>
       <c r="N53" s="13">
-        <f>SUM(N4:N52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O53" s="13">
-        <f>SUM(O4:O52)</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="P53" s="13">
-        <f>SUM(P4:P52)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="Q53" s="13">
-        <f>SUM(Q4:Q52)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="R53" s="13">
-        <f>SUM(R4:R52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S53" s="13">
-        <f>SUM(S4:S52)</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="T53" s="13">
-        <f>SUM(T4:T52)</f>
+        <f t="shared" si="1"/>
         <v>7.0059999999999993</v>
       </c>
       <c r="U53" s="13">
-        <f>SUM(U4:U52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V53" s="13">
-        <f>SUM(V4:V52)</f>
+        <f t="shared" si="1"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="W53" s="14">
-        <f>SUM(W4:W52)</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="X53" s="14">
-        <f>SUM(X4:X52)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.6800000000000002</v>
       </c>
       <c r="Y53" s="14">
-        <f>SUM(Y4:Y52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z53" s="14">
-        <f>SUM(Z4:Z52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA53" s="14">
-        <f>SUM(AA4:AA52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB53" s="14">
-        <f>SUM(AB4:AB52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC53" s="14">
-        <f>SUM(AC4:AC52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD53" s="14">
-        <f>SUM(AD4:AD52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE53" s="14">
-        <f>SUM(AE4:AE52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF53" s="14">
-        <f>SUM(AF4:AF52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG53" s="14">
-        <f>SUM(AG4:AG52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH53" s="14">
-        <f>SUM(AH4:AH52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI53" s="14">
-        <f>SUM(AI4:AI52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AJ53" s="14">
-        <f>SUM(AJ4:AJ52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AK53" s="14">
-        <f>SUM(AK4:AK52)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6650,36 +7201,36 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="123" t="s">
+      <c r="J54" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="K54" s="125"/>
-      <c r="L54" s="125"/>
-      <c r="M54" s="125"/>
-      <c r="N54" s="125"/>
-      <c r="O54" s="125"/>
-      <c r="P54" s="125"/>
-      <c r="Q54" s="125"/>
-      <c r="R54" s="125"/>
-      <c r="S54" s="125"/>
-      <c r="T54" s="125"/>
-      <c r="U54" s="125"/>
-      <c r="V54" s="125"/>
-      <c r="W54" s="125"/>
-      <c r="X54" s="125"/>
-      <c r="Y54" s="125"/>
-      <c r="Z54" s="125"/>
-      <c r="AA54" s="125"/>
-      <c r="AB54" s="125"/>
-      <c r="AC54" s="125"/>
-      <c r="AD54" s="125"/>
-      <c r="AE54" s="125"/>
-      <c r="AF54" s="125"/>
-      <c r="AG54" s="125"/>
-      <c r="AH54" s="125"/>
-      <c r="AI54" s="125"/>
-      <c r="AJ54" s="125"/>
-      <c r="AK54" s="132"/>
+      <c r="K54" s="127"/>
+      <c r="L54" s="127"/>
+      <c r="M54" s="127"/>
+      <c r="N54" s="127"/>
+      <c r="O54" s="127"/>
+      <c r="P54" s="127"/>
+      <c r="Q54" s="127"/>
+      <c r="R54" s="127"/>
+      <c r="S54" s="127"/>
+      <c r="T54" s="127"/>
+      <c r="U54" s="127"/>
+      <c r="V54" s="127"/>
+      <c r="W54" s="127"/>
+      <c r="X54" s="127"/>
+      <c r="Y54" s="127"/>
+      <c r="Z54" s="127"/>
+      <c r="AA54" s="127"/>
+      <c r="AB54" s="127"/>
+      <c r="AC54" s="127"/>
+      <c r="AD54" s="127"/>
+      <c r="AE54" s="127"/>
+      <c r="AF54" s="127"/>
+      <c r="AG54" s="127"/>
+      <c r="AH54" s="127"/>
+      <c r="AI54" s="127"/>
+      <c r="AJ54" s="127"/>
+      <c r="AK54" s="128"/>
     </row>
     <row r="55" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="19" t="s">
@@ -6723,10 +7274,10 @@
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="123" t="s">
+      <c r="H56" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="I56" s="124"/>
+      <c r="I56" s="153"/>
       <c r="J56" s="9">
         <f>H53-J53</f>
         <v>30.199999999999996</v>
@@ -6744,100 +7295,100 @@
         <v>29.734999999999996</v>
       </c>
       <c r="N56" s="9">
-        <f t="shared" ref="N56:W56" si="1">M56-N53</f>
+        <f t="shared" ref="N56:W56" si="2">M56-N53</f>
         <v>29.734999999999996</v>
       </c>
       <c r="O56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.434999999999995</v>
       </c>
       <c r="P56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.934999999999995</v>
       </c>
       <c r="Q56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.434999999999995</v>
       </c>
       <c r="R56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.434999999999995</v>
       </c>
       <c r="S56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28.384999999999994</v>
       </c>
       <c r="T56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.378999999999994</v>
       </c>
       <c r="U56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.378999999999994</v>
       </c>
       <c r="V56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.578999999999994</v>
       </c>
       <c r="W56" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.378999999999994</v>
       </c>
       <c r="X56" s="9">
-        <f t="shared" ref="X56" si="2">W56-X53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="X56" si="3">W56-X53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="Y56" s="9">
-        <f t="shared" ref="Y56" si="3">X56-Y53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="Y56" si="4">X56-Y53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="Z56" s="9">
-        <f t="shared" ref="Z56" si="4">Y56-Z53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="Z56" si="5">Y56-Z53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AA56" s="9">
-        <f t="shared" ref="AA56" si="5">Z56-AA53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AA56" si="6">Z56-AA53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AB56" s="9">
-        <f t="shared" ref="AB56" si="6">AA56-AB53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AB56" si="7">AA56-AB53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AC56" s="9">
-        <f t="shared" ref="AC56" si="7">AB56-AC53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AC56" si="8">AB56-AC53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AD56" s="9">
-        <f t="shared" ref="AD56" si="8">AC56-AD53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AD56" si="9">AC56-AD53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AE56" s="9">
-        <f t="shared" ref="AE56" si="9">AD56-AE53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AE56" si="10">AD56-AE53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AF56" s="9">
-        <f t="shared" ref="AF56" si="10">AE56-AF53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AF56" si="11">AE56-AF53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AG56" s="9">
-        <f t="shared" ref="AG56" si="11">AF56-AG53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AG56" si="12">AF56-AG53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AH56" s="9">
-        <f t="shared" ref="AH56" si="12">AG56-AH53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AH56" si="13">AG56-AH53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AI56" s="9">
-        <f t="shared" ref="AI56" si="13">AH56-AI53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AI56" si="14">AH56-AI53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AJ56" s="9">
-        <f t="shared" ref="AJ56" si="14">AI56-AJ53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AJ56" si="15">AI56-AJ53</f>
+        <v>16.698999999999995</v>
       </c>
       <c r="AK56" s="85">
-        <f t="shared" ref="AK56" si="15">AJ56-AK53</f>
-        <v>18.378999999999994</v>
+        <f t="shared" ref="AK56" si="16">AJ56-AK53</f>
+        <v>16.698999999999995</v>
       </c>
     </row>
     <row r="57" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6853,7 +7404,7 @@
         <v>4.2409999999999997</v>
       </c>
       <c r="E57" s="86">
-        <f t="shared" ref="E57:E58" si="16">SUM(C57,-D58)</f>
+        <f t="shared" ref="E57:E58" si="17">SUM(C57,-D58)</f>
         <v>5.4200000000000008</v>
       </c>
       <c r="F57" s="3"/>
@@ -6878,45 +7429,45 @@
         <v>2.2800000000000002</v>
       </c>
       <c r="E58" s="89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10.85</v>
       </c>
       <c r="F58" s="3"/>
-      <c r="H58" s="123" t="s">
+      <c r="H58" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="I58" s="125"/>
-      <c r="J58" s="123">
+      <c r="I58" s="127"/>
+      <c r="J58" s="126">
         <f>H53-I53</f>
         <v>18.378999999999991</v>
       </c>
-      <c r="K58" s="125"/>
-      <c r="L58" s="125"/>
-      <c r="M58" s="125"/>
-      <c r="N58" s="125"/>
-      <c r="O58" s="125"/>
-      <c r="P58" s="125"/>
-      <c r="Q58" s="125"/>
-      <c r="R58" s="125"/>
-      <c r="S58" s="125"/>
-      <c r="T58" s="125"/>
-      <c r="U58" s="125"/>
-      <c r="V58" s="125"/>
-      <c r="W58" s="125"/>
-      <c r="X58" s="125"/>
-      <c r="Y58" s="125"/>
-      <c r="Z58" s="125"/>
-      <c r="AA58" s="125"/>
-      <c r="AB58" s="125"/>
-      <c r="AC58" s="125"/>
-      <c r="AD58" s="125"/>
-      <c r="AE58" s="125"/>
-      <c r="AF58" s="125"/>
-      <c r="AG58" s="125"/>
-      <c r="AH58" s="125"/>
-      <c r="AI58" s="125"/>
-      <c r="AJ58" s="125"/>
-      <c r="AK58" s="132"/>
+      <c r="K58" s="127"/>
+      <c r="L58" s="127"/>
+      <c r="M58" s="127"/>
+      <c r="N58" s="127"/>
+      <c r="O58" s="127"/>
+      <c r="P58" s="127"/>
+      <c r="Q58" s="127"/>
+      <c r="R58" s="127"/>
+      <c r="S58" s="127"/>
+      <c r="T58" s="127"/>
+      <c r="U58" s="127"/>
+      <c r="V58" s="127"/>
+      <c r="W58" s="127"/>
+      <c r="X58" s="127"/>
+      <c r="Y58" s="127"/>
+      <c r="Z58" s="127"/>
+      <c r="AA58" s="127"/>
+      <c r="AB58" s="127"/>
+      <c r="AC58" s="127"/>
+      <c r="AD58" s="127"/>
+      <c r="AE58" s="127"/>
+      <c r="AF58" s="127"/>
+      <c r="AG58" s="127"/>
+      <c r="AH58" s="127"/>
+      <c r="AI58" s="127"/>
+      <c r="AJ58" s="127"/>
+      <c r="AK58" s="128"/>
     </row>
     <row r="59" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
@@ -6996,6 +7547,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="J58:AK58"/>
+    <mergeCell ref="J54:AK54"/>
     <mergeCell ref="J2:AK2"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="C22:C32"/>
@@ -7009,12 +7566,6 @@
     <mergeCell ref="C36:C40"/>
     <mergeCell ref="B17:B44"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="J58:AK58"/>
-    <mergeCell ref="J54:AK54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizado excel y añadida la espada blanca al dungeon.
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
+++ b/tabla scrum backlog + burndown chart - Sprint 5 SampleTextStudio.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iriag\Desktop\Alex\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -302,7 +302,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -965,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1311,10 +1311,49 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1368,12 +1407,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1392,37 +1425,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1445,7 +1448,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1663,10 +1666,10 @@
                   <c:v>10.808999999999996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.308999999999996</c:v>
+                  <c:v>9.3089999999999957</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.308999999999996</c:v>
+                  <c:v>8.8089999999999957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,6 +1736,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1789,7 +1793,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1864,23 +1868,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1916,23 +1903,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2108,14 +2078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:F37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG35" sqref="AG35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
     <col min="3" max="3" width="41.140625" customWidth="1"/>
@@ -2141,36 +2111,36 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="119" t="s">
+      <c r="J2" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="120"/>
-      <c r="AA2" s="120"/>
-      <c r="AB2" s="120"/>
-      <c r="AC2" s="120"/>
-      <c r="AD2" s="120"/>
-      <c r="AE2" s="120"/>
-      <c r="AF2" s="120"/>
-      <c r="AG2" s="120"/>
-      <c r="AH2" s="120"/>
-      <c r="AI2" s="120"/>
-      <c r="AJ2" s="120"/>
-      <c r="AK2" s="121"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="127"/>
+      <c r="W2" s="127"/>
+      <c r="X2" s="127"/>
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="134"/>
     </row>
     <row r="3" spans="1:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
@@ -2283,7 +2253,7 @@
       </c>
     </row>
     <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="147" t="s">
+      <c r="B4" s="128" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="32" t="s">
@@ -2392,7 +2362,7 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="138"/>
+      <c r="B5" s="129"/>
       <c r="C5" s="93" t="s">
         <v>85</v>
       </c>
@@ -2499,7 +2469,7 @@
       </c>
     </row>
     <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="139"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="26" t="s">
         <v>73</v>
       </c>
@@ -2606,7 +2576,7 @@
       </c>
     </row>
     <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="139"/>
+      <c r="B7" s="130"/>
       <c r="C7" s="26" t="s">
         <v>37</v>
       </c>
@@ -2713,7 +2683,7 @@
       </c>
     </row>
     <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="139"/>
+      <c r="B8" s="130"/>
       <c r="C8" s="26" t="s">
         <v>39</v>
       </c>
@@ -2818,7 +2788,7 @@
       </c>
     </row>
     <row r="9" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="148"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="45" t="s">
         <v>40</v>
       </c>
@@ -2925,7 +2895,7 @@
       </c>
     </row>
     <row r="10" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="155" t="s">
         <v>86</v>
       </c>
       <c r="C10" s="98" t="s">
@@ -3034,7 +3004,7 @@
       </c>
     </row>
     <row r="11" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="145"/>
+      <c r="B11" s="156"/>
       <c r="C11" s="105" t="s">
         <v>87</v>
       </c>
@@ -3250,10 +3220,10 @@
       </c>
     </row>
     <row r="13" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="142" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="49" t="s">
@@ -3361,8 +3331,8 @@
       </c>
     </row>
     <row r="14" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="139"/>
-      <c r="C14" s="130"/>
+      <c r="B14" s="130"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="34" t="s">
         <v>60</v>
       </c>
@@ -3468,8 +3438,8 @@
       </c>
     </row>
     <row r="15" spans="1:37" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="140"/>
-      <c r="C15" s="131"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="144"/>
       <c r="D15" s="54" t="s">
         <v>61</v>
       </c>
@@ -3682,10 +3652,10 @@
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="126" t="s">
+      <c r="B17" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="135" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="60" t="s">
@@ -3791,8 +3761,8 @@
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="127"/>
-      <c r="C18" s="123"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="136"/>
       <c r="D18" s="26" t="s">
         <v>75</v>
       </c>
@@ -3896,8 +3866,8 @@
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="127"/>
-      <c r="C19" s="123"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="136"/>
       <c r="D19" s="35" t="s">
         <v>50</v>
       </c>
@@ -4001,8 +3971,8 @@
       </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="127"/>
-      <c r="C20" s="123"/>
+      <c r="B20" s="140"/>
+      <c r="C20" s="136"/>
       <c r="D20" s="35" t="s">
         <v>33</v>
       </c>
@@ -4106,8 +4076,8 @@
       </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="127"/>
-      <c r="C21" s="123"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="136"/>
       <c r="D21" s="26" t="s">
         <v>34</v>
       </c>
@@ -4187,8 +4157,8 @@
       <c r="AK21" s="117"/>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="127"/>
-      <c r="C22" s="124" t="s">
+      <c r="B22" s="140"/>
+      <c r="C22" s="137" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="35" t="s">
@@ -4294,8 +4264,8 @@
       </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="127"/>
-      <c r="C23" s="124"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="137"/>
       <c r="D23" s="35" t="s">
         <v>45</v>
       </c>
@@ -4399,8 +4369,8 @@
       </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="127"/>
-      <c r="C24" s="124"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="137"/>
       <c r="D24" s="35" t="s">
         <v>46</v>
       </c>
@@ -4504,8 +4474,8 @@
       </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="127"/>
-      <c r="C25" s="124"/>
+      <c r="B25" s="140"/>
+      <c r="C25" s="137"/>
       <c r="D25" s="35" t="s">
         <v>47</v>
       </c>
@@ -4609,8 +4579,8 @@
       </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="127"/>
-      <c r="C26" s="124"/>
+      <c r="B26" s="140"/>
+      <c r="C26" s="137"/>
       <c r="D26" s="34" t="s">
         <v>48</v>
       </c>
@@ -4626,7 +4596,7 @@
       </c>
       <c r="I26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J26" s="82">
         <v>0</v>
@@ -4676,22 +4646,46 @@
       <c r="Y26" s="82">
         <v>0</v>
       </c>
-      <c r="Z26" s="29"/>
-      <c r="AA26" s="29"/>
-      <c r="AB26" s="29"/>
-      <c r="AC26" s="29"/>
-      <c r="AD26" s="29"/>
-      <c r="AE26" s="29"/>
-      <c r="AF26" s="29"/>
-      <c r="AG26" s="29"/>
-      <c r="AH26" s="30"/>
-      <c r="AI26" s="30"/>
-      <c r="AJ26" s="30"/>
-      <c r="AK26" s="31"/>
+      <c r="Z26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="82">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="157">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="114">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="127"/>
-      <c r="C27" s="124"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="137"/>
       <c r="D27" s="35" t="s">
         <v>51</v>
       </c>
@@ -4795,8 +4789,8 @@
       </c>
     </row>
     <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="127"/>
-      <c r="C28" s="124"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="137"/>
       <c r="D28" s="35" t="s">
         <v>52</v>
       </c>
@@ -4900,8 +4894,8 @@
       </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="127"/>
-      <c r="C29" s="124"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="137"/>
       <c r="D29" s="35" t="s">
         <v>53</v>
       </c>
@@ -5005,8 +4999,8 @@
       </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="127"/>
-      <c r="C30" s="124"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="137"/>
       <c r="D30" s="35" t="s">
         <v>57</v>
       </c>
@@ -5110,8 +5104,8 @@
       </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="127"/>
-      <c r="C31" s="124"/>
+      <c r="B31" s="140"/>
+      <c r="C31" s="137"/>
       <c r="D31" s="35" t="s">
         <v>55</v>
       </c>
@@ -5215,8 +5209,8 @@
       </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="127"/>
-      <c r="C32" s="124"/>
+      <c r="B32" s="140"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="35" t="s">
         <v>56</v>
       </c>
@@ -5320,8 +5314,8 @@
       </c>
     </row>
     <row r="33" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="127"/>
-      <c r="C33" s="125" t="s">
+      <c r="B33" s="140"/>
+      <c r="C33" s="138" t="s">
         <v>83</v>
       </c>
       <c r="D33" s="34" t="s">
@@ -5427,8 +5421,8 @@
       </c>
     </row>
     <row r="34" spans="2:37" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="127"/>
-      <c r="C34" s="125"/>
+      <c r="B34" s="140"/>
+      <c r="C34" s="138"/>
       <c r="D34" s="34" t="s">
         <v>54</v>
       </c>
@@ -5494,23 +5488,45 @@
       <c r="Y34" s="82">
         <v>0</v>
       </c>
-      <c r="Z34" s="29">
+      <c r="Z34" s="85">
         <v>0.73</v>
       </c>
-      <c r="AA34" s="29"/>
-      <c r="AB34" s="29"/>
-      <c r="AC34" s="29"/>
-      <c r="AD34" s="29"/>
-      <c r="AE34" s="29"/>
-      <c r="AF34" s="29"/>
-      <c r="AG34" s="29"/>
-      <c r="AH34" s="30"/>
-      <c r="AI34" s="30"/>
-      <c r="AJ34" s="30"/>
-      <c r="AK34" s="31"/>
+      <c r="AA34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="85">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="114">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="127"/>
+      <c r="B35" s="140"/>
       <c r="C35" s="39" t="s">
         <v>58</v>
       </c>
@@ -5615,8 +5631,8 @@
       </c>
     </row>
     <row r="36" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="127"/>
-      <c r="C36" s="141" t="s">
+      <c r="B36" s="140"/>
+      <c r="C36" s="152" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="35" t="s">
@@ -5698,8 +5714,8 @@
       <c r="AK36" s="31"/>
     </row>
     <row r="37" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="127"/>
-      <c r="C37" s="142"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="153"/>
       <c r="D37" s="26" t="s">
         <v>91</v>
       </c>
@@ -5803,8 +5819,8 @@
       </c>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="127"/>
-      <c r="C38" s="142"/>
+      <c r="B38" s="140"/>
+      <c r="C38" s="153"/>
       <c r="D38" s="34" t="s">
         <v>78</v>
       </c>
@@ -5908,8 +5924,8 @@
       </c>
     </row>
     <row r="39" spans="2:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="127"/>
-      <c r="C39" s="142"/>
+      <c r="B39" s="140"/>
+      <c r="C39" s="153"/>
       <c r="D39" s="34" t="s">
         <v>81</v>
       </c>
@@ -6013,8 +6029,8 @@
       </c>
     </row>
     <row r="40" spans="2:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="127"/>
-      <c r="C40" s="142"/>
+      <c r="B40" s="140"/>
+      <c r="C40" s="153"/>
       <c r="D40" s="34" t="s">
         <v>80</v>
       </c>
@@ -6118,8 +6134,8 @@
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="127"/>
-      <c r="C41" s="143"/>
+      <c r="B41" s="140"/>
+      <c r="C41" s="154"/>
       <c r="D41" s="34" t="s">
         <v>79</v>
       </c>
@@ -6223,8 +6239,8 @@
       </c>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="127"/>
-      <c r="C42" s="132" t="s">
+      <c r="B42" s="140"/>
+      <c r="C42" s="145" t="s">
         <v>62</v>
       </c>
       <c r="D42" s="34" t="s">
@@ -6322,16 +6338,16 @@
       <c r="AI42" s="82">
         <v>0</v>
       </c>
-      <c r="AJ42" s="151">
+      <c r="AJ42" s="119">
         <v>0.4</v>
       </c>
-      <c r="AK42" s="152">
+      <c r="AK42" s="120">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="127"/>
-      <c r="C43" s="132"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="145"/>
       <c r="D43" s="34" t="s">
         <v>64</v>
       </c>
@@ -6427,15 +6443,15 @@
       <c r="AI43" s="82">
         <v>0</v>
       </c>
-      <c r="AJ43" s="151">
+      <c r="AJ43" s="119">
         <v>0.1</v>
       </c>
-      <c r="AK43" s="152">
+      <c r="AK43" s="120">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="127"/>
+      <c r="B44" s="140"/>
       <c r="C44" s="38" t="s">
         <v>68</v>
       </c>
@@ -6540,7 +6556,7 @@
       </c>
     </row>
     <row r="45" spans="2:37" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="128"/>
+      <c r="B45" s="141"/>
       <c r="C45" s="61" t="s">
         <v>70</v>
       </c>
@@ -6607,37 +6623,37 @@
       <c r="Y45" s="89">
         <v>0</v>
       </c>
-      <c r="Z45" s="153">
+      <c r="Z45" s="121">
         <v>0.7</v>
       </c>
-      <c r="AA45" s="153">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="153">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="153">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="153">
-        <v>0</v>
-      </c>
-      <c r="AE45" s="153">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="153">
+      <c r="AA45" s="121">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="121">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="121">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="121">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="121">
+        <v>0</v>
+      </c>
+      <c r="AF45" s="121">
         <v>0</v>
       </c>
       <c r="AG45" s="111">
         <v>2.5</v>
       </c>
-      <c r="AH45" s="154"/>
-      <c r="AI45" s="154"/>
-      <c r="AJ45" s="154"/>
-      <c r="AK45" s="155"/>
+      <c r="AH45" s="122"/>
+      <c r="AI45" s="122"/>
+      <c r="AJ45" s="122"/>
+      <c r="AK45" s="123"/>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="133" t="s">
+      <c r="B46" s="146" t="s">
         <v>21</v>
       </c>
       <c r="C46" s="63" t="s">
@@ -6744,7 +6760,7 @@
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="134"/>
+      <c r="B47" s="147"/>
       <c r="C47" s="27" t="s">
         <v>27</v>
       </c>
@@ -6849,8 +6865,8 @@
       </c>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="134"/>
-      <c r="C48" s="136" t="s">
+      <c r="B48" s="147"/>
+      <c r="C48" s="149" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="26" t="s">
@@ -6956,8 +6972,8 @@
       </c>
     </row>
     <row r="49" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="135"/>
-      <c r="C49" s="137"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="150"/>
       <c r="D49" s="45" t="s">
         <v>24</v>
       </c>
@@ -7031,7 +7047,7 @@
       <c r="AK49" s="69"/>
     </row>
     <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="126" t="s">
+      <c r="B50" s="139" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="70" t="s">
@@ -7133,12 +7149,12 @@
       <c r="AJ50" s="85">
         <v>0</v>
       </c>
-      <c r="AK50" s="156">
+      <c r="AK50" s="124">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="127"/>
+      <c r="B51" s="140"/>
       <c r="C51" s="36" t="s">
         <v>82</v>
       </c>
@@ -7243,7 +7259,7 @@
       </c>
     </row>
     <row r="52" spans="2:37" ht="21" x14ac:dyDescent="0.25">
-      <c r="B52" s="127"/>
+      <c r="B52" s="140"/>
       <c r="C52" s="37" t="s">
         <v>66</v>
       </c>
@@ -7348,7 +7364,7 @@
       </c>
     </row>
     <row r="53" spans="2:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="128"/>
+      <c r="B53" s="141"/>
       <c r="C53" s="73" t="s">
         <v>67</v>
       </c>
@@ -7453,21 +7469,21 @@
       </c>
     </row>
     <row r="54" spans="2:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="149" t="s">
+      <c r="B54" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="150"/>
-      <c r="D54" s="150"/>
-      <c r="E54" s="150"/>
-      <c r="F54" s="150"/>
-      <c r="G54" s="150"/>
+      <c r="C54" s="133"/>
+      <c r="D54" s="133"/>
+      <c r="E54" s="133"/>
+      <c r="F54" s="133"/>
+      <c r="G54" s="133"/>
       <c r="H54" s="13">
         <f t="shared" ref="H54:AK54" si="2">SUM(H4:H53)</f>
         <v>30.299999999999997</v>
       </c>
       <c r="I54" s="13">
         <f t="shared" si="2"/>
-        <v>19.991000000000003</v>
+        <v>21.491000000000003</v>
       </c>
       <c r="J54" s="13">
         <f t="shared" si="2"/>
@@ -7575,11 +7591,11 @@
       </c>
       <c r="AJ54" s="14">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="AK54" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7591,36 +7607,36 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="119" t="s">
+      <c r="J55" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="K55" s="120"/>
-      <c r="L55" s="120"/>
-      <c r="M55" s="120"/>
-      <c r="N55" s="120"/>
-      <c r="O55" s="120"/>
-      <c r="P55" s="120"/>
-      <c r="Q55" s="120"/>
-      <c r="R55" s="120"/>
-      <c r="S55" s="120"/>
-      <c r="T55" s="120"/>
-      <c r="U55" s="120"/>
-      <c r="V55" s="120"/>
-      <c r="W55" s="120"/>
-      <c r="X55" s="120"/>
-      <c r="Y55" s="120"/>
-      <c r="Z55" s="120"/>
-      <c r="AA55" s="120"/>
-      <c r="AB55" s="120"/>
-      <c r="AC55" s="120"/>
-      <c r="AD55" s="120"/>
-      <c r="AE55" s="120"/>
-      <c r="AF55" s="120"/>
-      <c r="AG55" s="120"/>
-      <c r="AH55" s="120"/>
-      <c r="AI55" s="120"/>
-      <c r="AJ55" s="120"/>
-      <c r="AK55" s="121"/>
+      <c r="K55" s="127"/>
+      <c r="L55" s="127"/>
+      <c r="M55" s="127"/>
+      <c r="N55" s="127"/>
+      <c r="O55" s="127"/>
+      <c r="P55" s="127"/>
+      <c r="Q55" s="127"/>
+      <c r="R55" s="127"/>
+      <c r="S55" s="127"/>
+      <c r="T55" s="127"/>
+      <c r="U55" s="127"/>
+      <c r="V55" s="127"/>
+      <c r="W55" s="127"/>
+      <c r="X55" s="127"/>
+      <c r="Y55" s="127"/>
+      <c r="Z55" s="127"/>
+      <c r="AA55" s="127"/>
+      <c r="AB55" s="127"/>
+      <c r="AC55" s="127"/>
+      <c r="AD55" s="127"/>
+      <c r="AE55" s="127"/>
+      <c r="AF55" s="127"/>
+      <c r="AG55" s="127"/>
+      <c r="AH55" s="127"/>
+      <c r="AI55" s="127"/>
+      <c r="AJ55" s="127"/>
+      <c r="AK55" s="134"/>
     </row>
     <row r="56" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
@@ -7664,10 +7680,10 @@
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="119" t="s">
+      <c r="H57" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="I57" s="146"/>
+      <c r="I57" s="126"/>
       <c r="J57" s="9">
         <f>H54-J54</f>
         <v>30.299999999999997</v>
@@ -7774,11 +7790,11 @@
       </c>
       <c r="AJ57" s="9">
         <f t="shared" ref="AJ57" si="16">AI57-AJ54</f>
-        <v>10.308999999999996</v>
+        <v>9.3089999999999957</v>
       </c>
       <c r="AK57" s="76">
         <f t="shared" ref="AK57" si="17">AJ57-AK54</f>
-        <v>10.308999999999996</v>
+        <v>8.8089999999999957</v>
       </c>
     </row>
     <row r="58" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7816,48 +7832,48 @@
       </c>
       <c r="D59" s="79">
         <f>SUM(I13:I15,I33:I34,I38:I43,I45,I26)</f>
-        <v>10.350000000000001</v>
+        <v>11.850000000000001</v>
       </c>
       <c r="E59" s="80">
         <f>SUM(C59,-D59)</f>
-        <v>0.49999999999999822</v>
+        <v>-1.0000000000000018</v>
       </c>
       <c r="F59" s="3"/>
-      <c r="H59" s="119" t="s">
+      <c r="H59" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="I59" s="120"/>
-      <c r="J59" s="119">
+      <c r="I59" s="127"/>
+      <c r="J59" s="125">
         <f>H54-I54</f>
-        <v>10.308999999999994</v>
-      </c>
-      <c r="K59" s="120"/>
-      <c r="L59" s="120"/>
-      <c r="M59" s="120"/>
-      <c r="N59" s="120"/>
-      <c r="O59" s="120"/>
-      <c r="P59" s="120"/>
-      <c r="Q59" s="120"/>
-      <c r="R59" s="120"/>
-      <c r="S59" s="120"/>
-      <c r="T59" s="120"/>
-      <c r="U59" s="120"/>
-      <c r="V59" s="120"/>
-      <c r="W59" s="120"/>
-      <c r="X59" s="120"/>
-      <c r="Y59" s="120"/>
-      <c r="Z59" s="120"/>
-      <c r="AA59" s="120"/>
-      <c r="AB59" s="120"/>
-      <c r="AC59" s="120"/>
-      <c r="AD59" s="120"/>
-      <c r="AE59" s="120"/>
-      <c r="AF59" s="120"/>
-      <c r="AG59" s="120"/>
-      <c r="AH59" s="120"/>
-      <c r="AI59" s="120"/>
-      <c r="AJ59" s="120"/>
-      <c r="AK59" s="121"/>
+        <v>8.8089999999999939</v>
+      </c>
+      <c r="K59" s="127"/>
+      <c r="L59" s="127"/>
+      <c r="M59" s="127"/>
+      <c r="N59" s="127"/>
+      <c r="O59" s="127"/>
+      <c r="P59" s="127"/>
+      <c r="Q59" s="127"/>
+      <c r="R59" s="127"/>
+      <c r="S59" s="127"/>
+      <c r="T59" s="127"/>
+      <c r="U59" s="127"/>
+      <c r="V59" s="127"/>
+      <c r="W59" s="127"/>
+      <c r="X59" s="127"/>
+      <c r="Y59" s="127"/>
+      <c r="Z59" s="127"/>
+      <c r="AA59" s="127"/>
+      <c r="AB59" s="127"/>
+      <c r="AC59" s="127"/>
+      <c r="AD59" s="127"/>
+      <c r="AE59" s="127"/>
+      <c r="AF59" s="127"/>
+      <c r="AG59" s="127"/>
+      <c r="AH59" s="127"/>
+      <c r="AI59" s="127"/>
+      <c r="AJ59" s="127"/>
+      <c r="AK59" s="134"/>
     </row>
     <row r="60" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
@@ -7937,12 +7953,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="J59:AK59"/>
-    <mergeCell ref="J55:AK55"/>
     <mergeCell ref="J2:AK2"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="C22:C32"/>
@@ -7956,6 +7966,12 @@
     <mergeCell ref="C36:C41"/>
     <mergeCell ref="B17:B45"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="J59:AK59"/>
+    <mergeCell ref="J55:AK55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7964,24 +7980,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>